<commit_message>
added more updates to board count factor
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="502">
   <si>
     <t>Pass</t>
   </si>
@@ -1526,6 +1526,18 @@
   </si>
   <si>
     <t>Units Buying</t>
+  </si>
+  <si>
+    <t>MiniFit-6</t>
+  </si>
+  <si>
+    <t>16mhz</t>
+  </si>
+  <si>
+    <t>2u (2,2u)</t>
+  </si>
+  <si>
+    <t>850 (845)</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1665,39 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1963,12 +2007,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+      <selection pane="bottomLeft" activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,12 +2130,15 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
+      <c r="F5" s="4">
+        <v>77</v>
+      </c>
       <c r="G5">
-        <f>A5-F5</f>
-        <v>210</v>
+        <f t="shared" ref="G5:G36" si="0">A5-F5</f>
+        <v>133</v>
       </c>
       <c r="J5" s="4">
-        <f>H5*I5</f>
+        <f t="shared" ref="J5:J36" si="1">H5*I5</f>
         <v>0</v>
       </c>
     </row>
@@ -2109,12 +2156,15 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
+      <c r="F6" s="4">
+        <v>50</v>
+      </c>
       <c r="G6">
-        <f>A6-F6</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>-44</v>
       </c>
       <c r="J6" s="4">
-        <f>H6*I6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2132,12 +2182,15 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
+      <c r="F7" s="4">
+        <v>15</v>
+      </c>
       <c r="G7">
-        <f>A7-F7</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>-13</v>
       </c>
       <c r="J7" s="4">
-        <f>H7*I7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2155,12 +2208,15 @@
       <c r="D8" t="s">
         <v>9</v>
       </c>
+      <c r="F8" s="4">
+        <v>90</v>
+      </c>
       <c r="G8">
-        <f>A8-F8</f>
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>-60</v>
       </c>
       <c r="J8" s="4">
-        <f>H8*I8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2178,12 +2234,15 @@
       <c r="D9" t="s">
         <v>9</v>
       </c>
+      <c r="F9" s="4">
+        <v>100</v>
+      </c>
       <c r="G9">
-        <f>A9-F9</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>-98</v>
       </c>
       <c r="J9" s="4">
-        <f>H9*I9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2201,12 +2260,15 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
       <c r="G10">
-        <f>A10-F10</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J10" s="4">
-        <f>H10*I10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2224,12 +2286,15 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
+      <c r="F11" s="4">
+        <v>19</v>
+      </c>
       <c r="G11">
-        <f>A11-F11</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>-5</v>
       </c>
       <c r="J11" s="4">
-        <f>H11*I11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2247,12 +2312,15 @@
       <c r="D12" t="s">
         <v>182</v>
       </c>
+      <c r="F12" s="4">
+        <v>185</v>
+      </c>
       <c r="G12">
-        <f>A12-F12</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>-165</v>
       </c>
       <c r="J12" s="4">
-        <f>H12*I12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2270,12 +2338,15 @@
       <c r="D13" t="s">
         <v>182</v>
       </c>
+      <c r="F13" s="4">
+        <v>25</v>
+      </c>
       <c r="G13">
-        <f>A13-F13</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>-5</v>
       </c>
       <c r="J13" s="4">
-        <f>H13*I13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2293,12 +2364,15 @@
       <c r="D14" t="s">
         <v>182</v>
       </c>
+      <c r="F14" s="4">
+        <v>40</v>
+      </c>
       <c r="G14">
-        <f>A14-F14</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="J14" s="4">
-        <f>H14*I14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2316,12 +2390,15 @@
       <c r="D15" t="s">
         <v>9</v>
       </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
       <c r="G15">
-        <f>A15-F15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J15" s="4">
-        <f>H15*I15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2339,12 +2416,15 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
+      <c r="F16" s="4">
+        <v>54</v>
+      </c>
       <c r="G16">
-        <f>A16-F16</f>
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>-30</v>
       </c>
       <c r="J16" s="4">
-        <f>H16*I16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2362,12 +2442,15 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
+      <c r="F17" s="4">
+        <v>44</v>
+      </c>
       <c r="G17">
-        <f>A17-F17</f>
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>-18</v>
       </c>
       <c r="J17" s="4">
-        <f>H17*I17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2385,12 +2468,15 @@
       <c r="D18" t="s">
         <v>14</v>
       </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
       <c r="G18">
-        <f>A18-F18</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="J18" s="4">
-        <f>H18*I18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2408,12 +2494,15 @@
       <c r="D19" t="s">
         <v>14</v>
       </c>
+      <c r="F19" s="4">
+        <v>24</v>
+      </c>
       <c r="G19">
-        <f>A19-F19</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>-22</v>
       </c>
       <c r="J19" s="4">
-        <f>H19*I19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2423,7 +2512,7 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>500</v>
       </c>
       <c r="C20" t="s">
         <v>67</v>
@@ -2431,12 +2520,15 @@
       <c r="D20" t="s">
         <v>14</v>
       </c>
+      <c r="F20" s="4">
+        <v>20</v>
+      </c>
       <c r="G20">
-        <f>A20-F20</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>-16</v>
       </c>
       <c r="J20" s="4">
-        <f>H20*I20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2454,12 +2546,15 @@
       <c r="D21">
         <v>1206</v>
       </c>
+      <c r="F21" s="4">
+        <v>4</v>
+      </c>
       <c r="G21">
-        <f>A21-F21</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J21" s="4">
-        <f>H21*I21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2477,12 +2572,15 @@
       <c r="D22" t="s">
         <v>100</v>
       </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
       <c r="G22">
-        <f>A22-F22</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J22" s="4">
-        <f>H22*I22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2500,12 +2598,15 @@
       <c r="D23" t="s">
         <v>103</v>
       </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
       <c r="G23">
-        <f>A23-F23</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J23" s="4">
-        <f>H23*I23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2523,12 +2624,15 @@
       <c r="D24" t="s">
         <v>217</v>
       </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
       <c r="G24">
-        <f>A24-F24</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J24" s="4">
-        <f>H24*I24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2546,12 +2650,15 @@
       <c r="D25" t="s">
         <v>152</v>
       </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
       <c r="G25">
-        <f>A25-F25</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J25" s="4">
-        <f>H25*I25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2569,22 +2676,25 @@
       <c r="D26" t="s">
         <v>152</v>
       </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
       <c r="G26">
-        <f>A26-F26</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J26" s="4">
-        <f>H26*I26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>Laptimer!A28*BOM!B2+'Laptimer Remote'!A23*BOM!C2+'Com Node'!A27*BOM!D2+TC!A28*BOM!I2</f>
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>23</v>
+        <f>Dashboard!A21*BOM!E2</f>
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>15</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
@@ -2592,9 +2702,12 @@
       <c r="D27" t="s">
         <v>9</v>
       </c>
+      <c r="F27" s="4">
+        <v>50</v>
+      </c>
       <c r="G27">
         <f>A27-F27</f>
-        <v>35</v>
+        <v>-48</v>
       </c>
       <c r="J27" s="4">
         <f>H27*I27</f>
@@ -2603,11 +2716,11 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>Laptimer!A29*BOM!B2+'Laptimer Remote'!A24*BOM!C2</f>
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
+        <f>Laptimer!A33*BOM!B2+'Com Node'!A31*BOM!D2</f>
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>22</v>
       </c>
       <c r="C28" t="s">
         <v>68</v>
@@ -2615,9 +2728,12 @@
       <c r="D28" t="s">
         <v>9</v>
       </c>
+      <c r="F28" s="4">
+        <v>23</v>
+      </c>
       <c r="G28">
         <f>A28-F28</f>
-        <v>2</v>
+        <v>-15</v>
       </c>
       <c r="J28" s="4">
         <f>H28*I28</f>
@@ -2626,11 +2742,11 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>Laptimer!A30*BOM!B2+'Laptimer Remote'!A25*BOM!C2</f>
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
+        <f>'Com Node'!A36*BOM!D2+'CPU Board'!A25*BOM!F2+TC!A34*BOM!I2</f>
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>68</v>
@@ -2638,9 +2754,12 @@
       <c r="D29" t="s">
         <v>9</v>
       </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
       <c r="G29">
         <f>A29-F29</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="J29" s="4">
         <f>H29*I29</f>
@@ -2649,21 +2768,24 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>Laptimer!A31*BOM!B2+'Laptimer Remote'!A26*BOM!C2+'Com Node'!A28*BOM!D2+Dashboard!A22*BOM!E2+TC!A30*BOM!I2</f>
-        <v>20</v>
-      </c>
-      <c r="B30" t="s">
-        <v>26</v>
+        <f>'CPU Board'!A26*BOM!F2</f>
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>182</v>
+      </c>
+      <c r="F30" s="4">
+        <v>45</v>
       </c>
       <c r="G30">
         <f>A30-F30</f>
-        <v>20</v>
+        <v>-35</v>
       </c>
       <c r="J30" s="4">
         <f>H30*I30</f>
@@ -2672,11 +2794,11 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>Laptimer!A32*BOM!B2+'Laptimer Remote'!A27*BOM!C2</f>
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
+        <f>TC!A29*BOM!I2</f>
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>120</v>
       </c>
       <c r="C31" t="s">
         <v>68</v>
@@ -2684,9 +2806,12 @@
       <c r="D31" t="s">
         <v>9</v>
       </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
       <c r="G31">
         <f>A31-F31</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J31" s="4">
         <f>H31*I31</f>
@@ -2695,11 +2820,11 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>Laptimer!A33*BOM!B2+'Com Node'!A31*BOM!D2</f>
+        <f>Laptimer!A34*BOM!B2+'Laptimer Remote'!A28*BOM!C2</f>
         <v>8</v>
       </c>
       <c r="B32">
-        <v>22</v>
+        <v>220</v>
       </c>
       <c r="C32" t="s">
         <v>68</v>
@@ -2707,9 +2832,12 @@
       <c r="D32" t="s">
         <v>9</v>
       </c>
+      <c r="F32" s="4">
+        <v>50</v>
+      </c>
       <c r="G32">
         <f>A32-F32</f>
-        <v>8</v>
+        <v>-42</v>
       </c>
       <c r="J32" s="4">
         <f>H32*I32</f>
@@ -2718,17 +2846,20 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>Laptimer!A34*BOM!B2+'Laptimer Remote'!A28*BOM!C2</f>
+        <f>'Com Node'!A32*BOM!D2</f>
         <v>8</v>
       </c>
       <c r="B33">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="C33" t="s">
         <v>68</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
       </c>
       <c r="G33">
         <f>A33-F33</f>
@@ -2741,389 +2872,440 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
+        <f>Laptimer!A37*BOM!B2+'Laptimer Remote'!A31*BOM!C2+Relay!A10*BOM!G2</f>
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>470</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="4">
+        <v>24</v>
+      </c>
+      <c r="G34">
+        <f>A34-F34</f>
+        <v>-6</v>
+      </c>
+      <c r="J34" s="4">
+        <f>H34*I34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>Laptimer!A38*BOM!B2</f>
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>475</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f>A35-F35</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="4">
+        <f>H35*I35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>'Com Node'!A34*BOM!D2+TC!A32*BOM!I2</f>
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>499</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="4">
+        <v>17</v>
+      </c>
+      <c r="G36">
+        <f>A36-F36</f>
+        <v>-3</v>
+      </c>
+      <c r="J36" s="4">
+        <f>H36*I36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>'Com Node'!A35*BOM!D2+Dashboard!A24*BOM!E2+'CPU Board'!A27*BOM!F2+TC!A33*BOM!I2</f>
+        <v>82</v>
+      </c>
+      <c r="B37">
+        <v>500</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f>A37-F37</f>
+        <v>82</v>
+      </c>
+      <c r="J37" s="4">
+        <f>H37*I37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>'Com Node'!A37*BOM!D2</f>
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>501</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="4">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <f>A38-F38</f>
+        <v>-2</v>
+      </c>
+      <c r="J38" s="4">
+        <f>H38*I38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>Laptimer!A39*BOM!B2+Dashboard!A25*BOM!E2</f>
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>931</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f>A39-F39</f>
+        <v>9</v>
+      </c>
+      <c r="J39" s="4">
+        <f>H39*I39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>'Com Node'!A38*BOM!D2+TC!A35*BOM!I2</f>
+        <v>14</v>
+      </c>
+      <c r="B40">
+        <v>976</v>
+      </c>
+      <c r="C40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f>A40-F40</f>
+        <v>14</v>
+      </c>
+      <c r="J40" s="4">
+        <f>H40*I40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>Laptimer!A28*BOM!B2+'Laptimer Remote'!A23*BOM!C2+'Com Node'!A27*BOM!D2+TC!A28*BOM!I2</f>
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="4">
+        <v>48</v>
+      </c>
+      <c r="G41">
+        <f>A41-F41</f>
+        <v>-13</v>
+      </c>
+      <c r="J41" s="4">
+        <f>H41*I41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f>Laptimer!A29*BOM!B2+'Laptimer Remote'!A24*BOM!C2</f>
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="4">
+        <v>100</v>
+      </c>
+      <c r="G42">
+        <f>A42-F42</f>
+        <v>-98</v>
+      </c>
+      <c r="J42" s="4">
+        <f>H42*I42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>Laptimer!A30*BOM!B2+'Laptimer Remote'!A25*BOM!C2</f>
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="4">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <f>A43-F43</f>
+        <v>-8</v>
+      </c>
+      <c r="J43" s="4">
+        <f>H43*I43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f>Laptimer!A31*BOM!B2+'Laptimer Remote'!A26*BOM!C2+'Com Node'!A28*BOM!D2+Dashboard!A22*BOM!E2+TC!A30*BOM!I2</f>
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="4">
+        <v>30</v>
+      </c>
+      <c r="G44">
+        <f>A44-F44</f>
+        <v>-10</v>
+      </c>
+      <c r="J44" s="4">
+        <f>H44*I44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f>'Com Node'!A29*BOM!D2+Dashboard!A23*BOM!E2+TC!A31*BOM!I2</f>
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="4">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <f>A45-F45</f>
+        <v>-2</v>
+      </c>
+      <c r="J45" s="4">
+        <f>H45*I45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f>Laptimer!A32*BOM!B2+'Laptimer Remote'!A27*BOM!C2</f>
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f>A46-F46</f>
+        <v>2</v>
+      </c>
+      <c r="J46" s="4">
+        <f>H46*I46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f>'Com Node'!A30*BOM!D2</f>
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="4">
+        <v>24</v>
+      </c>
+      <c r="G47">
+        <f>A47-F47</f>
+        <v>-22</v>
+      </c>
+      <c r="J47" s="4">
+        <f>H47*I47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
         <f>Laptimer!A35*BOM!B2+'Laptimer Remote'!A29*BOM!C2</f>
         <v>3</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B48" t="s">
         <v>28</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C48" t="s">
         <v>68</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D48" t="s">
         <v>9</v>
       </c>
-      <c r="G34">
-        <f>A34-F34</f>
-        <v>3</v>
-      </c>
-      <c r="J34" s="4">
-        <f>H34*I34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="F48" s="4">
+        <v>25</v>
+      </c>
+      <c r="G48">
+        <f>A48-F48</f>
+        <v>-22</v>
+      </c>
+      <c r="J48" s="4">
+        <f>H48*I48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
         <f>Laptimer!A36*BOM!B2+'Laptimer Remote'!A30*BOM!C2</f>
         <v>2</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B49" t="s">
         <v>29</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C49" t="s">
         <v>68</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D49" t="s">
         <v>9</v>
       </c>
-      <c r="G35">
-        <f>A35-F35</f>
-        <v>2</v>
-      </c>
-      <c r="J35" s="4">
-        <f>H35*I35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f>Laptimer!A37*BOM!B2+'Laptimer Remote'!A31*BOM!C2+Relay!A10*BOM!G2</f>
-        <v>18</v>
-      </c>
-      <c r="B36">
-        <v>470</v>
-      </c>
-      <c r="C36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36">
-        <f>A36-F36</f>
-        <v>18</v>
-      </c>
-      <c r="J36" s="4">
-        <f>H36*I36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f>Laptimer!A38*BOM!B2</f>
-        <v>1</v>
-      </c>
-      <c r="B37">
-        <v>475</v>
-      </c>
-      <c r="C37" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37">
-        <f>A37-F37</f>
-        <v>1</v>
-      </c>
-      <c r="J37" s="4">
-        <f>H37*I37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f>Laptimer!A39*BOM!B2+Dashboard!A25*BOM!E2</f>
-        <v>9</v>
-      </c>
-      <c r="B38">
-        <v>931</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38">
-        <f>A38-F38</f>
-        <v>9</v>
-      </c>
-      <c r="J38" s="4">
-        <f>H38*I38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <f>'Com Node'!A29*BOM!D2+Dashboard!A23*BOM!E2+TC!A31*BOM!I2</f>
-        <v>6</v>
-      </c>
-      <c r="B39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39">
-        <f>A39-F39</f>
-        <v>6</v>
-      </c>
-      <c r="J39" s="4">
-        <f>H39*I39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <f>'Com Node'!A30*BOM!D2</f>
-        <v>2</v>
-      </c>
-      <c r="B40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40">
-        <f>A40-F40</f>
-        <v>2</v>
-      </c>
-      <c r="J40" s="4">
-        <f>H40*I40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f>'Com Node'!A32*BOM!D2</f>
-        <v>8</v>
-      </c>
-      <c r="B41">
-        <v>270</v>
-      </c>
-      <c r="C41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41">
-        <f>A41-F41</f>
-        <v>8</v>
-      </c>
-      <c r="J41" s="4">
-        <f>H41*I41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="F49" s="4">
+        <v>5</v>
+      </c>
+      <c r="G49">
+        <f>A49-F49</f>
+        <v>-3</v>
+      </c>
+      <c r="J49" s="4">
+        <f>H49*I49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
         <f>'Com Node'!A33*BOM!D2</f>
         <v>10</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B50" t="s">
         <v>127</v>
-      </c>
-      <c r="C42" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42">
-        <f>A42-F42</f>
-        <v>10</v>
-      </c>
-      <c r="J42" s="4">
-        <f>H42*I42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <f>'Com Node'!A34*BOM!D2+TC!A32*BOM!I2</f>
-        <v>14</v>
-      </c>
-      <c r="B43">
-        <v>499</v>
-      </c>
-      <c r="C43" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43">
-        <f>A43-F43</f>
-        <v>14</v>
-      </c>
-      <c r="J43" s="4">
-        <f>H43*I43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <f>'Com Node'!A35*BOM!D2+Dashboard!A24*BOM!E2+'CPU Board'!A27*BOM!F2+TC!A33*BOM!I2</f>
-        <v>82</v>
-      </c>
-      <c r="B44">
-        <v>500</v>
-      </c>
-      <c r="C44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44">
-        <f>A44-F44</f>
-        <v>82</v>
-      </c>
-      <c r="J44" s="4">
-        <f>H44*I44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f>'Com Node'!A36*BOM!D2+'CPU Board'!A25*BOM!F2+TC!A34*BOM!I2</f>
-        <v>28</v>
-      </c>
-      <c r="B45">
-        <v>60</v>
-      </c>
-      <c r="C45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45">
-        <f>A45-F45</f>
-        <v>28</v>
-      </c>
-      <c r="J45" s="4">
-        <f>H45*I45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f>'Com Node'!A37*BOM!D2</f>
-        <v>2</v>
-      </c>
-      <c r="B46">
-        <v>850</v>
-      </c>
-      <c r="C46" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46">
-        <f>A46-F46</f>
-        <v>2</v>
-      </c>
-      <c r="J46" s="4">
-        <f>H46*I46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <f>'Com Node'!A38*BOM!D2+TC!A35*BOM!I2</f>
-        <v>14</v>
-      </c>
-      <c r="B47">
-        <v>976</v>
-      </c>
-      <c r="C47" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47">
-        <f>A47-F47</f>
-        <v>14</v>
-      </c>
-      <c r="J47" s="4">
-        <f>H47*I47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f>'Com Node'!A39*BOM!D2</f>
-        <v>2</v>
-      </c>
-      <c r="B48" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48">
-        <f>A48-F48</f>
-        <v>2</v>
-      </c>
-      <c r="J48" s="4">
-        <f>H48*I48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f>Dashboard!A21*BOM!E2</f>
-        <v>2</v>
-      </c>
-      <c r="B49">
-        <v>15</v>
-      </c>
-      <c r="C49" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49">
-        <f>A49-F49</f>
-        <v>2</v>
-      </c>
-      <c r="J49" s="4">
-        <f>H49*I49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f>'CPU Board'!A26*BOM!F2</f>
-        <v>10</v>
-      </c>
-      <c r="B50">
-        <v>100</v>
       </c>
       <c r="C50" t="s">
         <v>68</v>
       </c>
       <c r="D50" t="s">
-        <v>182</v>
+        <v>9</v>
+      </c>
+      <c r="F50" s="4">
+        <v>25</v>
       </c>
       <c r="G50">
         <f>A50-F50</f>
-        <v>10</v>
+        <v>-15</v>
       </c>
       <c r="J50" s="4">
         <f>H50*I50</f>
@@ -3132,11 +3314,11 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f>TC!A29*BOM!I2</f>
-        <v>12</v>
-      </c>
-      <c r="B51">
-        <v>120</v>
+        <f>'Com Node'!A39*BOM!D2</f>
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>126</v>
       </c>
       <c r="C51" t="s">
         <v>68</v>
@@ -3146,7 +3328,7 @@
       </c>
       <c r="G51">
         <f>A51-F51</f>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J51" s="4">
         <f>H51*I51</f>
@@ -3166,11 +3348,11 @@
         <v>14</v>
       </c>
       <c r="G52">
-        <f>A52-F52</f>
+        <f t="shared" ref="G37:G68" si="2">A52-F52</f>
         <v>8</v>
       </c>
       <c r="J52" s="4">
-        <f>H52*I52</f>
+        <f t="shared" ref="J37:J68" si="3">H52*I52</f>
         <v>0</v>
       </c>
     </row>
@@ -3188,12 +3370,15 @@
       <c r="D53" t="s">
         <v>14</v>
       </c>
+      <c r="F53" s="4">
+        <v>0</v>
+      </c>
       <c r="G53">
-        <f>A53-F53</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J53" s="4">
-        <f>H53*I53</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3211,12 +3396,15 @@
       <c r="D54" t="s">
         <v>14</v>
       </c>
+      <c r="F54" s="4">
+        <v>59</v>
+      </c>
       <c r="G54">
-        <f>A54-F54</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>-57</v>
       </c>
       <c r="J54" s="4">
-        <f>H54*I54</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3234,12 +3422,15 @@
       <c r="D55" t="s">
         <v>70</v>
       </c>
+      <c r="F55" s="4">
+        <v>0</v>
+      </c>
       <c r="G55">
-        <f>A55-F55</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J55" s="4">
-        <f>H55*I55</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3257,12 +3448,15 @@
       <c r="D56" t="s">
         <v>14</v>
       </c>
+      <c r="F56" s="4">
+        <v>3</v>
+      </c>
       <c r="G56">
-        <f>A56-F56</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>-2</v>
       </c>
       <c r="J56" s="4">
-        <f>H56*I56</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3280,12 +3474,15 @@
       <c r="D57" t="s">
         <v>21</v>
       </c>
+      <c r="F57" s="4">
+        <v>0</v>
+      </c>
       <c r="G57">
-        <f>A57-F57</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J57" s="4">
-        <f>H57*I57</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3301,12 +3498,15 @@
       <c r="D58">
         <v>1206</v>
       </c>
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
       <c r="G58">
-        <f>A58-F58</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J58" s="4">
-        <f>H58*I58</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3322,12 +3522,15 @@
       <c r="D59" t="s">
         <v>123</v>
       </c>
+      <c r="F59" s="4">
+        <v>0</v>
+      </c>
       <c r="G59">
-        <f>A59-F59</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J59" s="4">
-        <f>H59*I59</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3345,12 +3548,15 @@
       <c r="D60" t="s">
         <v>109</v>
       </c>
+      <c r="F60" s="4">
+        <v>3</v>
+      </c>
       <c r="G60">
-        <f>A60-F60</f>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="J60" s="4">
-        <f>H60*I60</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3368,12 +3574,15 @@
       <c r="D61" t="s">
         <v>109</v>
       </c>
+      <c r="F61" s="4">
+        <v>5</v>
+      </c>
       <c r="G61">
-        <f>A61-F61</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>-3</v>
       </c>
       <c r="J61" s="4">
-        <f>H61*I61</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3391,12 +3600,15 @@
       <c r="D62" t="s">
         <v>136</v>
       </c>
+      <c r="F62" s="4">
+        <v>1</v>
+      </c>
       <c r="G62">
-        <f>A62-F62</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="J62" s="4">
-        <f>H62*I62</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3414,12 +3626,15 @@
       <c r="D63" t="s">
         <v>172</v>
       </c>
+      <c r="F63" s="4">
+        <v>1</v>
+      </c>
       <c r="G63">
-        <f>A63-F63</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="J63" s="4">
-        <f>H63*I63</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3479,6 +3694,9 @@
       <c r="D67" t="s">
         <v>72</v>
       </c>
+      <c r="F67" s="4">
+        <v>0</v>
+      </c>
       <c r="G67">
         <f>A67-F67</f>
         <v>6</v>
@@ -3502,12 +3720,15 @@
       <c r="D68" t="s">
         <v>36</v>
       </c>
+      <c r="F68" s="4">
+        <v>100</v>
+      </c>
       <c r="G68">
-        <f t="shared" ref="G68:G72" si="0">A68-F68</f>
-        <v>1</v>
+        <f t="shared" ref="G68:G72" si="4">A68-F68</f>
+        <v>-99</v>
       </c>
       <c r="J68" s="4">
-        <f t="shared" ref="J68:J72" si="1">H68*I68</f>
+        <f t="shared" ref="J68:J72" si="5">H68*I68</f>
         <v>0</v>
       </c>
     </row>
@@ -3525,12 +3746,15 @@
       <c r="D69" t="s">
         <v>38</v>
       </c>
+      <c r="F69" s="4">
+        <v>0</v>
+      </c>
       <c r="G69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J69" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3548,12 +3772,15 @@
       <c r="D70" t="s">
         <v>41</v>
       </c>
+      <c r="F70" s="4">
+        <v>20</v>
+      </c>
       <c r="G70">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>-18</v>
       </c>
       <c r="J70" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3571,12 +3798,15 @@
       <c r="D71" t="s">
         <v>43</v>
       </c>
+      <c r="F71" s="4">
+        <v>20</v>
+      </c>
       <c r="G71">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>-18</v>
       </c>
       <c r="J71" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3594,12 +3824,15 @@
       <c r="D72" t="s">
         <v>38</v>
       </c>
+      <c r="F72" s="4">
+        <v>0</v>
+      </c>
       <c r="G72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J72" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3617,12 +3850,15 @@
       <c r="D73" t="s">
         <v>90</v>
       </c>
+      <c r="F73" s="4">
+        <v>45</v>
+      </c>
       <c r="G73">
-        <f t="shared" ref="G73:G75" si="2">A73-F73</f>
-        <v>2</v>
+        <f t="shared" ref="G73:G75" si="6">A73-F73</f>
+        <v>-43</v>
       </c>
       <c r="J73" s="4">
-        <f t="shared" ref="J73:J75" si="3">H73*I73</f>
+        <f t="shared" ref="J73:J75" si="7">H73*I73</f>
         <v>0</v>
       </c>
     </row>
@@ -3638,12 +3874,15 @@
       <c r="D74" t="s">
         <v>111</v>
       </c>
+      <c r="F74" s="4">
+        <v>29</v>
+      </c>
       <c r="G74">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="J74" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3659,12 +3898,15 @@
       <c r="D75" t="s">
         <v>113</v>
       </c>
+      <c r="F75" s="4">
+        <v>0</v>
+      </c>
       <c r="G75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="J75" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3682,12 +3924,15 @@
       <c r="D76" t="s">
         <v>135</v>
       </c>
+      <c r="F76" s="4">
+        <v>0</v>
+      </c>
       <c r="G76">
-        <f t="shared" ref="G76:G78" si="4">A76-F76</f>
+        <f t="shared" ref="G76:G78" si="8">A76-F76</f>
         <v>2</v>
       </c>
       <c r="J76" s="4">
-        <f t="shared" ref="J76:J78" si="5">H76*I76</f>
+        <f t="shared" ref="J76:J78" si="9">H76*I76</f>
         <v>0</v>
       </c>
     </row>
@@ -3703,12 +3948,15 @@
       <c r="D77" t="s">
         <v>43</v>
       </c>
+      <c r="F77" s="4">
+        <v>13</v>
+      </c>
       <c r="G77">
-        <f t="shared" si="4"/>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>-1</v>
       </c>
       <c r="J77" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3724,12 +3972,15 @@
       <c r="D78" t="s">
         <v>141</v>
       </c>
+      <c r="F78" s="4">
+        <v>0</v>
+      </c>
       <c r="G78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="J78" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3745,12 +3996,15 @@
       <c r="D79" t="s">
         <v>143</v>
       </c>
+      <c r="F79" s="4">
+        <v>0</v>
+      </c>
       <c r="G79">
-        <f t="shared" ref="G79" si="6">A79-F79</f>
+        <f t="shared" ref="G79" si="10">A79-F79</f>
         <v>4</v>
       </c>
       <c r="J79" s="4">
-        <f t="shared" ref="J79" si="7">H79*I79</f>
+        <f t="shared" ref="J79" si="11">H79*I79</f>
         <v>0</v>
       </c>
     </row>
@@ -3768,12 +4022,15 @@
       <c r="D80" t="s">
         <v>164</v>
       </c>
+      <c r="F80" s="4">
+        <v>10</v>
+      </c>
       <c r="G80">
-        <f t="shared" ref="G80" si="8">A80-F80</f>
-        <v>2</v>
+        <f t="shared" ref="G80" si="12">A80-F80</f>
+        <v>-8</v>
       </c>
       <c r="J80" s="4">
-        <f t="shared" ref="J80" si="9">H80*I80</f>
+        <f t="shared" ref="J80" si="13">H80*I80</f>
         <v>0</v>
       </c>
     </row>
@@ -3791,12 +4048,15 @@
       <c r="D81" t="s">
         <v>223</v>
       </c>
+      <c r="F81" s="4">
+        <v>0</v>
+      </c>
       <c r="G81">
-        <f t="shared" ref="G81:G82" si="10">A81-F81</f>
+        <f t="shared" ref="G81:G82" si="14">A81-F81</f>
         <v>12</v>
       </c>
       <c r="J81" s="4">
-        <f t="shared" ref="J81:J82" si="11">H81*I81</f>
+        <f t="shared" ref="J81:J82" si="15">H81*I81</f>
         <v>0</v>
       </c>
     </row>
@@ -3812,12 +4072,15 @@
       <c r="D82" t="s">
         <v>230</v>
       </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
       <c r="G82">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="J82" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3865,484 +4128,567 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f>Laptimer!A2*BOM!B2</f>
-        <v>1</v>
+        <f>Dashboard!A4*BOM!E2</f>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="C86" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="D86" t="s">
-        <v>47</v>
+        <v>150</v>
+      </c>
+      <c r="F86" s="4">
+        <v>0</v>
       </c>
       <c r="G86">
         <f>A86-F86</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J86" s="4">
-        <f>J111</f>
+        <f>H86*I86</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f>Laptimer!A21*BOM!B2+'Laptimer Remote'!A16*BOM!C2</f>
+        <f>TC!A4*BOM!I2</f>
         <v>2</v>
       </c>
       <c r="B87" t="s">
-        <v>48</v>
+        <v>226</v>
       </c>
       <c r="C87" t="s">
-        <v>48</v>
+        <v>226</v>
       </c>
       <c r="D87" t="s">
-        <v>49</v>
+        <v>225</v>
+      </c>
+      <c r="F87" s="4">
+        <v>0</v>
       </c>
       <c r="G87">
-        <f t="shared" ref="G87:G89" si="12">A87-F87</f>
+        <f>A87-F87</f>
         <v>2</v>
       </c>
       <c r="J87" s="4">
-        <f t="shared" ref="J87:J89" si="13">H87*I87</f>
+        <f>H87*I87</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f>Laptimer!A22*BOM!B2+'Laptimer Remote'!A17*BOM!C2</f>
-        <v>2</v>
+        <f>'Com Node'!A4*BOM!D2</f>
+        <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="C88" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="D88" t="s">
-        <v>51</v>
+        <v>93</v>
+      </c>
+      <c r="F88" s="4">
+        <v>0</v>
       </c>
       <c r="G88">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <f>A88-F88</f>
+        <v>8</v>
       </c>
       <c r="J88" s="4">
-        <f t="shared" si="13"/>
+        <f>H88*I88</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
+        <f>Laptimer!A2*BOM!B2</f>
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>46</v>
+      </c>
+      <c r="C89" t="s">
+        <v>46</v>
+      </c>
+      <c r="D89" t="s">
+        <v>47</v>
+      </c>
+      <c r="F89" s="4">
+        <v>3</v>
+      </c>
+      <c r="G89">
+        <f>A89-F89</f>
+        <v>-2</v>
+      </c>
+      <c r="J89" s="4">
+        <f>J114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f>Dashboard!A13*BOM!E2</f>
+        <v>2</v>
+      </c>
+      <c r="B90" t="s">
+        <v>162</v>
+      </c>
+      <c r="C90" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" t="s">
+        <v>160</v>
+      </c>
+      <c r="F90" s="4">
+        <v>4</v>
+      </c>
+      <c r="G90">
+        <f>A90-F90</f>
+        <v>-2</v>
+      </c>
+      <c r="J90" s="4">
+        <f>H90*I90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f>TC!A16*BOM!I2</f>
+        <v>2</v>
+      </c>
+      <c r="B91" t="s">
+        <v>233</v>
+      </c>
+      <c r="C91" t="s">
+        <v>233</v>
+      </c>
+      <c r="D91" t="s">
+        <v>232</v>
+      </c>
+      <c r="F91" s="4">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <f>A91-F91</f>
+        <v>2</v>
+      </c>
+      <c r="J91" s="4">
+        <f>H91*I91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f>'Com Node'!A21*BOM!D2+Dashboard!A16*BOM!E2+TC!A18*BOM!I2</f>
+        <v>6</v>
+      </c>
+      <c r="B92" t="s">
+        <v>114</v>
+      </c>
+      <c r="C92" t="s">
+        <v>115</v>
+      </c>
+      <c r="D92" t="s">
+        <v>116</v>
+      </c>
+      <c r="F92" s="4">
+        <v>6</v>
+      </c>
+      <c r="G92">
+        <f>A92-F92</f>
+        <v>0</v>
+      </c>
+      <c r="J92" s="4">
+        <f>H92*I92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f>'Laptimer Remote'!A15*BOM!C2</f>
+        <v>1</v>
+      </c>
+      <c r="B93"/>
+      <c r="C93" t="s">
+        <v>86</v>
+      </c>
+      <c r="D93" t="s">
+        <v>87</v>
+      </c>
+      <c r="F93" s="4">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <f>A93-F93</f>
+        <v>1</v>
+      </c>
+      <c r="J93" s="4">
+        <f>H93*I93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f>Laptimer!A21*BOM!B2+'Laptimer Remote'!A16*BOM!C2</f>
+        <v>2</v>
+      </c>
+      <c r="B94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C94" t="s">
+        <v>48</v>
+      </c>
+      <c r="D94" t="s">
+        <v>49</v>
+      </c>
+      <c r="F94" s="4">
+        <v>2</v>
+      </c>
+      <c r="G94">
+        <f>A94-F94</f>
+        <v>0</v>
+      </c>
+      <c r="J94" s="4">
+        <f>H94*I94</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f>'Com Node'!A22*BOM!D2+'CPU Board'!A16*BOM!F2+TC!A19*BOM!I2</f>
+        <v>14</v>
+      </c>
+      <c r="B95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C95" t="s">
+        <v>117</v>
+      </c>
+      <c r="D95" t="s">
+        <v>118</v>
+      </c>
+      <c r="F95" s="4">
+        <v>4</v>
+      </c>
+      <c r="G95">
+        <f>A95-F95</f>
+        <v>10</v>
+      </c>
+      <c r="J95" s="4">
+        <f>H95*I95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f>'Com Node'!A23*BOM!D2+TC!A20*BOM!I2</f>
+        <v>4</v>
+      </c>
+      <c r="B96" t="s">
+        <v>119</v>
+      </c>
+      <c r="C96" t="s">
+        <v>119</v>
+      </c>
+      <c r="D96" t="s">
+        <v>120</v>
+      </c>
+      <c r="F96" s="4">
+        <v>8</v>
+      </c>
+      <c r="G96">
+        <f>A96-F96</f>
+        <v>-4</v>
+      </c>
+      <c r="J96" s="4">
+        <f>H96*I96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f>TC!A21*BOM!I2</f>
+        <v>4</v>
+      </c>
+      <c r="B97" t="s">
+        <v>240</v>
+      </c>
+      <c r="C97" t="s">
+        <v>239</v>
+      </c>
+      <c r="D97" t="s">
+        <v>238</v>
+      </c>
+      <c r="F97" s="4">
+        <v>2</v>
+      </c>
+      <c r="G97">
+        <f>A97-F97</f>
+        <v>2</v>
+      </c>
+      <c r="J97" s="4">
+        <f>H97*I97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f>'Com Node'!A24*BOM!D2</f>
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>121</v>
+      </c>
+      <c r="C98" t="s">
+        <v>121</v>
+      </c>
+      <c r="D98" t="s">
+        <v>122</v>
+      </c>
+      <c r="F98" s="4">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <f>A98-F98</f>
+        <v>4</v>
+      </c>
+      <c r="J98" s="4">
+        <f>H98*I98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <f>TC!A22*BOM!I2</f>
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>237</v>
+      </c>
+      <c r="C99" t="s">
+        <v>237</v>
+      </c>
+      <c r="D99" t="s">
+        <v>236</v>
+      </c>
+      <c r="F99" s="4">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <f>A99-F99</f>
+        <v>2</v>
+      </c>
+      <c r="J99" s="4">
+        <f>H99*I99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f>TC!A23*BOM!I2</f>
+        <v>30</v>
+      </c>
+      <c r="B100" t="s">
+        <v>235</v>
+      </c>
+      <c r="C100" t="s">
+        <v>235</v>
+      </c>
+      <c r="D100" t="s">
+        <v>234</v>
+      </c>
+      <c r="F100" s="4">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <f>A100-F100</f>
+        <v>30</v>
+      </c>
+      <c r="J100" s="4">
+        <f>H100*I100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <f>Laptimer!A22*BOM!B2+'Laptimer Remote'!A17*BOM!C2</f>
+        <v>2</v>
+      </c>
+      <c r="B101" t="s">
+        <v>50</v>
+      </c>
+      <c r="C101" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" t="s">
+        <v>51</v>
+      </c>
+      <c r="F101" s="4">
+        <v>9</v>
+      </c>
+      <c r="G101">
+        <f>A101-F101</f>
+        <v>-7</v>
+      </c>
+      <c r="J101" s="4">
+        <f>H101*I101</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102">
         <f>Laptimer!A27*BOM!B2+'Laptimer Remote'!A22*BOM!C2+'CPU Board'!A24*BOM!F2</f>
         <v>12</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B102" t="s">
         <v>52</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C102" t="s">
         <v>125</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D102" t="s">
         <v>53</v>
       </c>
-      <c r="G89">
-        <f t="shared" si="12"/>
-        <v>12</v>
-      </c>
-      <c r="J89" s="4">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="F102" s="4">
+        <v>5</v>
+      </c>
+      <c r="G102">
+        <f>A102-F102</f>
+        <v>7</v>
+      </c>
+      <c r="J102" s="4">
+        <f>H102*I102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103">
         <f>'Com Node'!A26*BOM!D2+'H-bridge'!A8*BOM!H2+TC!A27*BOM!I2</f>
         <v>6</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B103" t="s">
         <v>52</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C103" t="s">
         <v>124</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D103" t="s">
         <v>53</v>
       </c>
-      <c r="G90">
-        <f t="shared" ref="G90:G97" si="14">A90-F90</f>
-        <v>6</v>
-      </c>
-      <c r="J90" s="4">
-        <f t="shared" ref="J90:J97" si="15">H90*I90</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>0</v>
-      </c>
-      <c r="B91"/>
-      <c r="C91" t="s">
-        <v>86</v>
-      </c>
-      <c r="D91" t="s">
-        <v>87</v>
-      </c>
-      <c r="G91">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J91" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>0</v>
-      </c>
-      <c r="B92" t="s">
-        <v>94</v>
-      </c>
-      <c r="C92" t="s">
-        <v>94</v>
-      </c>
-      <c r="D92" t="s">
-        <v>93</v>
-      </c>
-      <c r="G92">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J92" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>0</v>
-      </c>
-      <c r="B93" t="s">
-        <v>114</v>
-      </c>
-      <c r="C93" t="s">
-        <v>115</v>
-      </c>
-      <c r="D93" t="s">
-        <v>116</v>
-      </c>
-      <c r="G93">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>0</v>
-      </c>
-      <c r="B94" t="s">
-        <v>117</v>
-      </c>
-      <c r="C94" t="s">
-        <v>117</v>
-      </c>
-      <c r="D94" t="s">
-        <v>118</v>
-      </c>
-      <c r="G94">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J94" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>0</v>
-      </c>
-      <c r="B95" t="s">
-        <v>119</v>
-      </c>
-      <c r="C95" t="s">
-        <v>119</v>
-      </c>
-      <c r="D95" t="s">
-        <v>120</v>
-      </c>
-      <c r="G95">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J95" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>0</v>
-      </c>
-      <c r="B96" t="s">
-        <v>121</v>
-      </c>
-      <c r="C96" t="s">
-        <v>121</v>
-      </c>
-      <c r="D96" t="s">
-        <v>122</v>
-      </c>
-      <c r="G96">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J96" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>0</v>
-      </c>
-      <c r="B97" t="s">
-        <v>151</v>
-      </c>
-      <c r="C97" t="s">
-        <v>151</v>
-      </c>
-      <c r="D97" t="s">
-        <v>150</v>
-      </c>
-      <c r="G97">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J97" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>0</v>
-      </c>
-      <c r="B98" t="s">
-        <v>162</v>
-      </c>
-      <c r="C98" t="s">
-        <v>161</v>
-      </c>
-      <c r="D98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G98">
-        <f t="shared" ref="G98:G99" si="16">A98-F98</f>
-        <v>0</v>
-      </c>
-      <c r="J98" s="4">
-        <f t="shared" ref="J98:J99" si="17">H98*I98</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>0</v>
-      </c>
-      <c r="B99" t="s">
-        <v>171</v>
-      </c>
-      <c r="C99" t="s">
-        <v>171</v>
-      </c>
-      <c r="D99" t="s">
-        <v>170</v>
-      </c>
-      <c r="G99">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J99" s="4">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>0</v>
-      </c>
-      <c r="B100"/>
-      <c r="C100" t="s">
-        <v>203</v>
-      </c>
-      <c r="D100" t="s">
-        <v>202</v>
-      </c>
-      <c r="G100">
-        <f t="shared" ref="G100" si="18">A100-F100</f>
-        <v>0</v>
-      </c>
-      <c r="J100" s="4">
-        <f t="shared" ref="J100" si="19">H100*I100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>0</v>
-      </c>
-      <c r="B101" t="s">
-        <v>222</v>
-      </c>
-      <c r="C101" t="s">
-        <v>222</v>
-      </c>
-      <c r="D101" t="s">
-        <v>222</v>
-      </c>
-      <c r="G101">
-        <f t="shared" ref="G101:G103" si="20">A101-F101</f>
-        <v>0</v>
-      </c>
-      <c r="J101" s="4">
-        <f t="shared" ref="J101:J103" si="21">H101*I101</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>0</v>
-      </c>
-      <c r="B102" t="s">
-        <v>226</v>
-      </c>
-      <c r="C102" t="s">
-        <v>226</v>
-      </c>
-      <c r="D102" t="s">
-        <v>225</v>
-      </c>
-      <c r="G102">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="J102" s="4">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>0</v>
-      </c>
-      <c r="B103" t="s">
-        <v>233</v>
-      </c>
-      <c r="C103" t="s">
-        <v>233</v>
-      </c>
-      <c r="D103" t="s">
-        <v>232</v>
+      <c r="F103" s="4">
+        <v>4</v>
       </c>
       <c r="G103">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f>A103-F103</f>
+        <v>2</v>
       </c>
       <c r="J103" s="4">
-        <f t="shared" si="21"/>
+        <f>H103*I103</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>0</v>
-      </c>
-      <c r="B104" t="s">
-        <v>240</v>
-      </c>
+        <f>'CPU Board'!A28*BOM!F2</f>
+        <v>10</v>
+      </c>
+      <c r="B104"/>
       <c r="C104" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="D104" t="s">
-        <v>238</v>
+        <v>202</v>
+      </c>
+      <c r="F104" s="4">
+        <v>6</v>
       </c>
       <c r="G104">
-        <f t="shared" ref="G104:G106" si="22">A104-F104</f>
-        <v>0</v>
+        <f>A104-F104</f>
+        <v>4</v>
       </c>
       <c r="J104" s="4">
-        <f t="shared" ref="J104:J106" si="23">H104*I104</f>
+        <f>H104*I104</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>0</v>
+        <f>Dashboard!A29*BOM!E2</f>
+        <v>8</v>
       </c>
       <c r="B105" t="s">
-        <v>237</v>
+        <v>171</v>
       </c>
       <c r="C105" t="s">
-        <v>237</v>
+        <v>171</v>
       </c>
       <c r="D105" t="s">
-        <v>236</v>
+        <v>170</v>
+      </c>
+      <c r="F105" s="4">
+        <v>4</v>
       </c>
       <c r="G105">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f>A105-F105</f>
+        <v>4</v>
       </c>
       <c r="J105" s="4">
-        <f t="shared" si="23"/>
+        <f>H105*I105</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>0</v>
-      </c>
-      <c r="B106" t="s">
-        <v>235</v>
-      </c>
+        <f>TC!A42*BOM!I2</f>
+        <v>2</v>
+      </c>
+      <c r="B106"/>
       <c r="C106" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="D106" t="s">
-        <v>234</v>
+        <v>243</v>
+      </c>
+      <c r="F106" s="4">
+        <v>0</v>
       </c>
       <c r="G106">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f>A106-F106</f>
+        <v>2</v>
       </c>
       <c r="J106" s="4">
-        <f t="shared" si="23"/>
+        <f>H106*I106</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>0</v>
-      </c>
-      <c r="B107"/>
+        <f>'H-bridge'!A10*BOM!H2</f>
+        <v>4</v>
+      </c>
+      <c r="B107" t="s">
+        <v>222</v>
+      </c>
       <c r="C107" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
       <c r="D107" t="s">
-        <v>243</v>
+        <v>222</v>
+      </c>
+      <c r="F107" s="4">
+        <v>0</v>
       </c>
       <c r="G107">
-        <f t="shared" ref="G107" si="24">A107-F107</f>
-        <v>0</v>
+        <f>A107-F107</f>
+        <v>4</v>
       </c>
       <c r="J107" s="4">
-        <f t="shared" ref="J107" si="25">H107*I107</f>
+        <f>H107*I107</f>
         <v>0</v>
       </c>
     </row>
@@ -4390,7 +4736,8 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>0</v>
+        <f>Laptimer!A3*BOM!B2</f>
+        <v>1</v>
       </c>
       <c r="B111" t="s">
         <v>76</v>
@@ -4401,9 +4748,12 @@
       <c r="D111" t="s">
         <v>76</v>
       </c>
+      <c r="F111" s="4">
+        <v>0</v>
+      </c>
       <c r="G111">
         <f>A111-F111</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" s="4">
         <f>H111*I111</f>
@@ -4412,7 +4762,8 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>0</v>
+        <f>Laptimer!A4*BOM!B2+'Laptimer Remote'!A2*BOM!C2</f>
+        <v>2</v>
       </c>
       <c r="B112"/>
       <c r="C112" t="s">
@@ -4421,18 +4772,22 @@
       <c r="D112" t="s">
         <v>74</v>
       </c>
+      <c r="F112" s="4">
+        <v>10</v>
+      </c>
       <c r="G112">
-        <f t="shared" ref="G112:G116" si="26">A112-F112</f>
-        <v>0</v>
+        <f t="shared" ref="G112:G115" si="16">A112-F112</f>
+        <v>-8</v>
       </c>
       <c r="J112" s="4">
-        <f t="shared" ref="J112:J116" si="27">H112*I112</f>
+        <f t="shared" ref="J112:J115" si="17">H112*I112</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>0</v>
+        <f>Laptimer!A23*BOM!B2+'Laptimer Remote'!A18*BOM!C2+'CPU Board'!A18*BOM!F2</f>
+        <v>12</v>
       </c>
       <c r="B113" t="s">
         <v>56</v>
@@ -4443,912 +4798,954 @@
       <c r="D113" t="s">
         <v>57</v>
       </c>
+      <c r="F113" s="4">
+        <v>8</v>
+      </c>
       <c r="G113">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>4</v>
       </c>
       <c r="J113" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>0</v>
-      </c>
-      <c r="B114"/>
+        <f>Laptimer!A41*BOM!B2+'CPU Board'!A30*BOM!F2</f>
+        <v>11</v>
+      </c>
+      <c r="B114" t="s">
+        <v>80</v>
+      </c>
       <c r="C114" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D114" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="G114">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>11</v>
       </c>
       <c r="J114" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>0</v>
+        <f>Laptimer!A42*BOM!B2+'Laptimer Remote'!A33*BOM!C2</f>
+        <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C115" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="D115" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G115">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>2</v>
       </c>
       <c r="J115" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>0</v>
+        <f>'Com Node'!A16*BOM!D2</f>
+        <v>2</v>
       </c>
       <c r="B116" t="s">
-        <v>58</v>
-      </c>
-      <c r="C116" t="s">
-        <v>58</v>
+        <v>105</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="D116" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="G116">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" ref="G116:G118" si="18">A116-F116</f>
+        <v>2</v>
       </c>
       <c r="J116" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="J116:J118" si="19">H116*I116</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>0</v>
+        <f>'Com Node'!A40*BOM!D2</f>
+        <v>2</v>
       </c>
       <c r="B117" t="s">
-        <v>105</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>106</v>
+        <v>130</v>
+      </c>
+      <c r="C117" t="s">
+        <v>130</v>
       </c>
       <c r="D117" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="G117">
-        <f t="shared" ref="G117:G119" si="28">A117-F117</f>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>2</v>
       </c>
       <c r="J117" s="4">
-        <f t="shared" ref="J117:J119" si="29">H117*I117</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>0</v>
-      </c>
-      <c r="B118" t="s">
-        <v>130</v>
-      </c>
+        <f>'Com Node'!A41*BOM!D2</f>
+        <v>2</v>
+      </c>
+      <c r="B118"/>
       <c r="C118" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D118" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G118">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>2</v>
       </c>
       <c r="J118" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>0</v>
-      </c>
-      <c r="B119"/>
+        <f>'Com Node'!A44*BOM!D2</f>
+        <v>2</v>
+      </c>
+      <c r="B119" t="s">
+        <v>137</v>
+      </c>
       <c r="C119" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D119" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G119">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" ref="G119:G121" si="20">A119-F119</f>
+        <v>2</v>
       </c>
       <c r="J119" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="J119:J121" si="21">H119*I119</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>0</v>
+        <f>Dashboard!A2*BOM!E2</f>
+        <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C120" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D120" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G120">
-        <f t="shared" ref="G120:G122" si="30">A120-F120</f>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>12</v>
       </c>
       <c r="J120" s="4">
-        <f t="shared" ref="J120:J122" si="31">H120*I120</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>0</v>
+        <f>Dashboard!A30*BOM!E2</f>
+        <v>2</v>
       </c>
       <c r="B121" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C121" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D121" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="G121">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>2</v>
       </c>
       <c r="J121" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>0</v>
+        <f>Dashboard!A3*BOM!E2</f>
+        <v>2</v>
       </c>
       <c r="B122" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C122" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D122" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G122">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f>A122-F122</f>
+        <v>2</v>
       </c>
       <c r="J122" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="J122" si="22">H122*I122</f>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>0</v>
+        <f>Dashboard!A18*BOM!E2</f>
+        <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C123" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="D123" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="G123">
         <f>A123-F123</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J123" s="4">
-        <f t="shared" ref="J123" si="32">H123*I123</f>
+        <f t="shared" ref="J123" si="23">H123*I123</f>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>0</v>
+        <f>'CPU Board'!A2*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="C124" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D124" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="G124">
-        <f>A124-F124</f>
-        <v>0</v>
+        <f t="shared" ref="G124:G129" si="24">A124-F124</f>
+        <v>10</v>
       </c>
       <c r="J124" s="4">
-        <f t="shared" ref="J124" si="33">H124*I124</f>
+        <f t="shared" ref="J124:J129" si="25">H124*I124</f>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>0</v>
+        <f>'CPU Board'!A3*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B125" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C125" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D125" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G125">
-        <f t="shared" ref="G125:G131" si="34">A125-F125</f>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>10</v>
       </c>
       <c r="J125" s="4">
-        <f t="shared" ref="J125:J131" si="35">H125*I125</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>0</v>
+        <f>'CPU Board'!A17*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B126" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C126" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="D126" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="G126">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>10</v>
       </c>
       <c r="J126" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>0</v>
-      </c>
-      <c r="B127" t="s">
-        <v>192</v>
-      </c>
+        <f>'CPU Board'!A20*BOM!F2</f>
+        <v>20</v>
+      </c>
+      <c r="B127"/>
       <c r="C127" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D127" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="G127">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>20</v>
       </c>
       <c r="J127" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>0</v>
+        <f>'CPU Board'!A21*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B128"/>
       <c r="C128" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D128" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G128">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>10</v>
       </c>
       <c r="J128" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>0</v>
+        <f>'CPU Board'!A22*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B129"/>
       <c r="C129" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D129" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G129">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>10</v>
       </c>
       <c r="J129" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>0</v>
-      </c>
-      <c r="B130"/>
+        <f>'CPU Board'!A29*BOM!F2+TC!A39*BOM!I2</f>
+        <v>18</v>
+      </c>
+      <c r="B130" t="s">
+        <v>205</v>
+      </c>
       <c r="C130" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="D130" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="G130">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" ref="G130:G131" si="26">A130-F130</f>
+        <v>18</v>
       </c>
       <c r="J130" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="J130:J131" si="27">H130*I130</f>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>0</v>
+        <f>'CPU Board'!A31*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B131"/>
       <c r="C131" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="D131" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="G131">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>10</v>
       </c>
       <c r="J131" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>0</v>
+        <f>Relay!A2*BOM!G2</f>
+        <v>4</v>
       </c>
       <c r="B132" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C132" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D132" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="G132">
-        <f t="shared" ref="G132:G133" si="36">A132-F132</f>
-        <v>0</v>
+        <f t="shared" ref="G132:G136" si="28">A132-F132</f>
+        <v>4</v>
       </c>
       <c r="J132" s="4">
-        <f t="shared" ref="J132:J133" si="37">H132*I132</f>
+        <f t="shared" ref="J132:J136" si="29">H132*I132</f>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>0</v>
-      </c>
-      <c r="B133"/>
+        <f>Relay!A3*BOM!G2</f>
+        <v>2</v>
+      </c>
+      <c r="B133" t="s">
+        <v>215</v>
+      </c>
       <c r="C133" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D133" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="G133">
-        <f t="shared" si="36"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>2</v>
       </c>
       <c r="J133" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>0</v>
+        <f>Relay!A4*BOM!G2</f>
+        <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>215</v>
+        <v>498</v>
       </c>
       <c r="C134" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D134" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G134">
-        <f t="shared" ref="G134:G138" si="38">A134-F134</f>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>2</v>
       </c>
       <c r="J134" s="4">
-        <f t="shared" ref="J134:J138" si="39">H134*I134</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>0</v>
+        <f>Relay!A6*BOM!G2</f>
+        <v>8</v>
       </c>
       <c r="B135" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C135" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D135" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="G135">
-        <f t="shared" si="38"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>8</v>
       </c>
       <c r="J135" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>0</v>
+        <f>Relay!A8*BOM!G2</f>
+        <v>8</v>
       </c>
       <c r="B136" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C136" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D136" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G136">
-        <f t="shared" si="38"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>8</v>
       </c>
       <c r="J136" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>0</v>
+        <f>'H-bridge'!A2*BOM!H2</f>
+        <v>2</v>
       </c>
       <c r="B137" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C137" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D137" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G137">
-        <f t="shared" si="38"/>
-        <v>0</v>
+        <f t="shared" ref="G137:G140" si="30">A137-F137</f>
+        <v>2</v>
       </c>
       <c r="J137" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="J137:J140" si="31">H137*I137</f>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>0</v>
+        <f>'H-bridge'!A7*BOM!H2</f>
+        <v>8</v>
       </c>
       <c r="B138" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="C138" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D138" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="G138">
-        <f t="shared" si="38"/>
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>8</v>
       </c>
       <c r="J138" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>0</v>
+        <f>TC!A5*BOM!I2</f>
+        <v>4</v>
       </c>
       <c r="B139" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="C139" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="D139" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="G139">
-        <f t="shared" ref="G139:G142" si="40">A139-F139</f>
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>4</v>
       </c>
       <c r="J139" s="4">
-        <f t="shared" ref="J139:J142" si="41">H139*I139</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>0</v>
       </c>
       <c r="B140" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C140" t="s">
-        <v>221</v>
+        <v>79</v>
       </c>
       <c r="D140" t="s">
-        <v>220</v>
+        <v>78</v>
       </c>
       <c r="G140">
-        <f t="shared" si="40"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J140" s="4">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>0</v>
-      </c>
-      <c r="B141" t="s">
-        <v>228</v>
-      </c>
-      <c r="C141" t="s">
-        <v>227</v>
-      </c>
-      <c r="D141" t="s">
-        <v>227</v>
-      </c>
-      <c r="G141">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J141" s="4">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>0</v>
-      </c>
-      <c r="B142" t="s">
-        <v>241</v>
-      </c>
-      <c r="C142" t="s">
-        <v>79</v>
-      </c>
-      <c r="D142" t="s">
-        <v>78</v>
-      </c>
-      <c r="G142">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J142" s="4">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I143" s="4" t="s">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I141" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J143" s="6">
-        <f>SUM(J111:J116)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="145" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A145" s="3" t="s">
+      <c r="J141" s="6">
+        <f>SUM(J111:J115)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:10" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A143" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B145" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D145" s="3" t="s">
+      <c r="B143" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D143" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E145" s="3" t="s">
+      <c r="E143" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F145" s="3" t="s">
+      <c r="F143" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G145" s="2" t="s">
+      <c r="G143" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H145" s="3" t="s">
+      <c r="H143" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I145" s="3" t="s">
+      <c r="I143" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J145" s="3" t="s">
+      <c r="J143" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <f>Laptimer!A15*BOM!B2</f>
+        <v>1</v>
+      </c>
+      <c r="B144" t="s">
+        <v>499</v>
+      </c>
+      <c r="C144" t="s">
+        <v>61</v>
+      </c>
+      <c r="D144" t="s">
+        <v>62</v>
+      </c>
+      <c r="F144" s="4">
+        <v>4</v>
+      </c>
+      <c r="G144">
+        <f>A144-F144</f>
+        <v>-3</v>
+      </c>
+      <c r="J144" s="4">
+        <f>H144*I144</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <f>Laptimer!A19*BOM!B2+'Laptimer Remote'!A13*BOM!C2+'Com Node'!A17*BOM!D2</f>
+        <v>4</v>
+      </c>
+      <c r="B145" t="s">
+        <v>82</v>
+      </c>
+      <c r="C145" t="s">
+        <v>82</v>
+      </c>
+      <c r="D145" t="s">
+        <v>81</v>
+      </c>
+      <c r="F145" s="4">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <f t="shared" ref="G145:G147" si="32">A145-F145</f>
+        <v>4</v>
+      </c>
+      <c r="J145" s="4">
+        <f t="shared" ref="J145:J147" si="33">H145*I145</f>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>0</v>
+        <f>Laptimer!A45*BOM!B2+'Com Node'!A47*BOM!D2</f>
+        <v>3</v>
       </c>
       <c r="B146" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C146" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D146" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="F146" s="4">
+        <v>2</v>
       </c>
       <c r="G146">
-        <f>A146-F146</f>
-        <v>0</v>
+        <f t="shared" si="32"/>
+        <v>1</v>
       </c>
       <c r="J146" s="4">
-        <f>H146*I146</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>0</v>
-      </c>
-      <c r="B147" t="s">
-        <v>82</v>
-      </c>
-      <c r="C147" t="s">
-        <v>82</v>
-      </c>
-      <c r="D147" t="s">
-        <v>81</v>
+        <f>'Com Node'!A2*BOM!D2</f>
+        <v>2</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F147" s="4">
+        <v>0</v>
       </c>
       <c r="G147">
-        <f t="shared" ref="G147:G149" si="42">A147-F147</f>
-        <v>0</v>
+        <f t="shared" si="32"/>
+        <v>2</v>
       </c>
       <c r="J147" s="4">
-        <f t="shared" ref="J147:J149" si="43">H147*I147</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>0</v>
+        <f>'Com Node'!A15*BOM!D2</f>
+        <v>4</v>
       </c>
       <c r="B148" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="C148" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D148" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="F148" s="4">
+        <v>0</v>
       </c>
       <c r="G148">
-        <f t="shared" si="42"/>
-        <v>0</v>
+        <f>A148-F148</f>
+        <v>4</v>
       </c>
       <c r="J148" s="4">
-        <f t="shared" si="43"/>
+        <f>H148*I148</f>
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>0</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D149" s="4" t="s">
-        <v>89</v>
+        <f>Dashboard!A12*BOM!E2</f>
+        <v>2</v>
+      </c>
+      <c r="B149" t="s">
+        <v>158</v>
+      </c>
+      <c r="C149" t="s">
+        <v>158</v>
+      </c>
+      <c r="D149" t="s">
+        <v>158</v>
+      </c>
+      <c r="F149" s="4">
+        <v>0</v>
       </c>
       <c r="G149">
-        <f t="shared" si="42"/>
-        <v>0</v>
+        <f t="shared" ref="G149:G150" si="34">A149-F149</f>
+        <v>2</v>
       </c>
       <c r="J149" s="4">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="J149:J150" si="35">H149*I149</f>
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>0</v>
+        <f>A149</f>
+        <v>2</v>
       </c>
       <c r="B150" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
       <c r="C150" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="D150" t="s">
-        <v>62</v>
+        <v>158</v>
+      </c>
+      <c r="F150" s="4">
+        <v>0</v>
       </c>
       <c r="G150">
-        <f>A150-F150</f>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>2</v>
       </c>
       <c r="J150" s="4">
-        <f>H150*I150</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>0</v>
+        <f>'CPU Board'!A13*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B151" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="C151" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="D151" t="s">
-        <v>158</v>
+        <v>187</v>
+      </c>
+      <c r="E151"/>
+      <c r="F151" s="9">
+        <v>1</v>
       </c>
       <c r="G151">
-        <f t="shared" ref="G151:G152" si="44">A151-F151</f>
-        <v>0</v>
+        <f t="shared" ref="G151" si="36">A151-F151</f>
+        <v>9</v>
       </c>
       <c r="J151" s="4">
-        <f t="shared" ref="J151:J152" si="45">H151*I151</f>
+        <f t="shared" ref="J151" si="37">H151*I151</f>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>0</v>
+        <f>'CPU Board'!A14*BOM!F2</f>
+        <v>10</v>
       </c>
       <c r="B152" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="C152" t="s">
-        <v>158</v>
+        <v>189</v>
       </c>
       <c r="D152" t="s">
-        <v>158</v>
+        <v>190</v>
+      </c>
+      <c r="F152" s="4">
+        <v>7</v>
       </c>
       <c r="G152">
-        <f t="shared" si="44"/>
-        <v>0</v>
+        <f t="shared" ref="G152" si="38">A152-F152</f>
+        <v>3</v>
       </c>
       <c r="J152" s="4">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>0</v>
-      </c>
-      <c r="B153" t="s">
-        <v>185</v>
-      </c>
-      <c r="C153" t="s">
-        <v>186</v>
-      </c>
-      <c r="D153" t="s">
-        <v>187</v>
-      </c>
-      <c r="E153"/>
-      <c r="F153"/>
-      <c r="G153">
-        <f t="shared" ref="G153" si="46">A153-F153</f>
-        <v>0</v>
-      </c>
-      <c r="J153" s="4">
-        <f t="shared" ref="J153" si="47">H153*I153</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>0</v>
-      </c>
-      <c r="B154" t="s">
-        <v>188</v>
-      </c>
-      <c r="C154" t="s">
-        <v>189</v>
-      </c>
-      <c r="D154" t="s">
-        <v>190</v>
-      </c>
-      <c r="G154">
-        <f t="shared" ref="G154" si="48">A154-F154</f>
-        <v>0</v>
-      </c>
-      <c r="J154" s="4">
-        <f t="shared" ref="J154" si="49">H154*I154</f>
-        <v>0</v>
-      </c>
-    </row>
+        <f t="shared" ref="J152" si="39">H152*I152</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I153" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J153" s="6">
+        <f>SUM(J144:J152)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="155" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I155" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J155" s="6">
-        <f>SUM(J146:J154)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J157" s="7">
-        <f>J155+J143+J108+J83+J64</f>
-        <v>0</v>
-      </c>
-      <c r="K157" t="s">
+      <c r="J155" s="7">
+        <f>J153+J141+J108+J83+J64</f>
+        <v>0</v>
+      </c>
+      <c r="K155" t="s">
         <v>245</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A86:J107">
+    <sortCondition ref="C86:C107"/>
+  </sortState>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6243,6 +6640,12 @@
       </c>
       <c r="F45" t="s">
         <v>316</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <f>TC!A16*Laptimer!I2</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6945,7 +7348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -8495,7 +8898,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9548,7 +9951,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
last update to instock
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="506">
   <si>
     <t>Pass</t>
   </si>
@@ -1538,6 +1538,18 @@
   </si>
   <si>
     <t>850 (845)</t>
+  </si>
+  <si>
+    <t>AUTOCONNECTOR-header</t>
+  </si>
+  <si>
+    <t>RELAY</t>
+  </si>
+  <si>
+    <t>RELAY 30A</t>
+  </si>
+  <si>
+    <t>MiniFit-6-header</t>
   </si>
 </sst>
 </file>
@@ -1665,7 +1677,44 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -2007,12 +2056,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K155"/>
+  <dimension ref="A1:K159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F153" sqref="F153"/>
+      <selection pane="bottomLeft" activeCell="B124" sqref="B124:D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2121,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G2" s="9">
         <v>2</v>
@@ -2119,7 +2168,7 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>Laptimer!A6*BOM!B2+'Laptimer Remote'!A4*BOM!C2+'Com Node'!A5*BOM!D2+BOM!E2*Dashboard!A5+'CPU Board'!A5*BOM!F2+BOM!I2*TC!A6</f>
-        <v>210</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -2134,11 +2183,11 @@
         <v>77</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G36" si="0">A5-F5</f>
-        <v>133</v>
+        <f t="shared" ref="G5:G26" si="0">A5-F5</f>
+        <v>173</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J36" si="1">H5*I5</f>
+        <f t="shared" ref="J5:J26" si="1">H5*I5</f>
         <v>0</v>
       </c>
     </row>
@@ -2197,7 +2246,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>Laptimer!A9*BOM!B2+'Com Node'!A6*BOM!D2+'CPU Board'!A8*BOM!F2</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>65</v>
@@ -2213,7 +2262,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>-60</v>
+        <v>-50</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="1"/>
@@ -2275,7 +2324,7 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>'Com Node'!A11*BOM!D2+'CPU Board'!A4*BOM!F2+TC!A9*BOM!I2</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>97</v>
@@ -2291,7 +2340,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="1"/>
@@ -2301,7 +2350,7 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>'CPU Board'!A10*BOM!F2</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>180</v>
@@ -2317,7 +2366,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>-165</v>
+        <v>-155</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="1"/>
@@ -2327,7 +2376,7 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>'CPU Board'!A11*BOM!F2</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>183</v>
@@ -2343,7 +2392,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="1"/>
@@ -2353,7 +2402,7 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>'CPU Board'!A12*BOM!F2</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>184</v>
@@ -2369,7 +2418,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="1"/>
@@ -2405,7 +2454,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>Laptimer!A11*BOM!B2+'Laptimer Remote'!A8*BOM!C2+'Com Node'!A8*BOM!D2+'CPU Board'!A6*BOM!F2+'H-bridge'!A3*BOM!H2+TC!A10*BOM!I2</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -2421,7 +2470,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>-30</v>
+        <v>-25</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="1"/>
@@ -2431,7 +2480,7 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>Laptimer!A12*BOM!B2+'Com Node'!A9*BOM!D2+Dashboard!A6*BOM!E2+'CPU Board'!A7*BOM!F2</f>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -2447,7 +2496,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>-18</v>
+        <v>-8</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="1"/>
@@ -2457,7 +2506,7 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>Laptimer!A13*BOM!B2+'Laptimer Remote'!A9*BOM!C2+'Com Node'!A10*BOM!D2+'CPU Board'!A9*BOM!F2+'H-bridge'!A4*BOM!H2+TC!A11*BOM!I2</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -2473,7 +2522,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="1"/>
@@ -2706,11 +2755,11 @@
         <v>50</v>
       </c>
       <c r="G27">
-        <f>A27-F27</f>
+        <f t="shared" ref="G27:G51" si="2">A27-F27</f>
         <v>-48</v>
       </c>
       <c r="J27" s="4">
-        <f>H27*I27</f>
+        <f t="shared" ref="J27:J51" si="3">H27*I27</f>
         <v>0</v>
       </c>
     </row>
@@ -2732,18 +2781,18 @@
         <v>23</v>
       </c>
       <c r="G28">
-        <f>A28-F28</f>
+        <f t="shared" si="2"/>
         <v>-15</v>
       </c>
       <c r="J28" s="4">
-        <f>H28*I28</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>'Com Node'!A36*BOM!D2+'CPU Board'!A25*BOM!F2+TC!A34*BOM!I2</f>
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>60</v>
@@ -2758,18 +2807,18 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <f>A29-F29</f>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="J29" s="4">
-        <f>H29*I29</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>'CPU Board'!A26*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B30">
         <v>100</v>
@@ -2784,11 +2833,11 @@
         <v>45</v>
       </c>
       <c r="G30">
-        <f>A30-F30</f>
-        <v>-35</v>
+        <f t="shared" si="2"/>
+        <v>-30</v>
       </c>
       <c r="J30" s="4">
-        <f>H30*I30</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2810,11 +2859,11 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <f>A31-F31</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J31" s="4">
-        <f>H31*I31</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2836,11 +2885,11 @@
         <v>50</v>
       </c>
       <c r="G32">
-        <f>A32-F32</f>
+        <f t="shared" si="2"/>
         <v>-42</v>
       </c>
       <c r="J32" s="4">
-        <f>H32*I32</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2862,11 +2911,11 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <f>A33-F33</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="J33" s="4">
-        <f>H33*I33</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2888,11 +2937,11 @@
         <v>24</v>
       </c>
       <c r="G34">
-        <f>A34-F34</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="J34" s="4">
-        <f>H34*I34</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2914,11 +2963,11 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <f>A35-F35</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J35" s="4">
-        <f>H35*I35</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2940,18 +2989,18 @@
         <v>17</v>
       </c>
       <c r="G36">
-        <f>A36-F36</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="J36" s="4">
-        <f>H36*I36</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>'Com Node'!A35*BOM!D2+Dashboard!A24*BOM!E2+'CPU Board'!A27*BOM!F2+TC!A33*BOM!I2</f>
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B37">
         <v>500</v>
@@ -2966,11 +3015,11 @@
         <v>0</v>
       </c>
       <c r="G37">
-        <f>A37-F37</f>
-        <v>82</v>
+        <f t="shared" si="2"/>
+        <v>92</v>
       </c>
       <c r="J37" s="4">
-        <f>H37*I37</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2992,11 +3041,11 @@
         <v>4</v>
       </c>
       <c r="G38">
-        <f>A38-F38</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="J38" s="4">
-        <f>H38*I38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3018,11 +3067,11 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <f>A39-F39</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J39" s="4">
-        <f>H39*I39</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3044,11 +3093,11 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <f>A40-F40</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J40" s="4">
-        <f>H40*I40</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3070,11 +3119,11 @@
         <v>48</v>
       </c>
       <c r="G41">
-        <f>A41-F41</f>
+        <f t="shared" si="2"/>
         <v>-13</v>
       </c>
       <c r="J41" s="4">
-        <f>H41*I41</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3096,11 +3145,11 @@
         <v>100</v>
       </c>
       <c r="G42">
-        <f>A42-F42</f>
+        <f t="shared" si="2"/>
         <v>-98</v>
       </c>
       <c r="J42" s="4">
-        <f>H42*I42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3122,11 +3171,11 @@
         <v>10</v>
       </c>
       <c r="G43">
-        <f>A43-F43</f>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="J43" s="4">
-        <f>H43*I43</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3148,11 +3197,11 @@
         <v>30</v>
       </c>
       <c r="G44">
-        <f>A44-F44</f>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="J44" s="4">
-        <f>H44*I44</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3174,11 +3223,11 @@
         <v>8</v>
       </c>
       <c r="G45">
-        <f>A45-F45</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="J45" s="4">
-        <f>H45*I45</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3200,11 +3249,11 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <f>A46-F46</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J46" s="4">
-        <f>H46*I46</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3226,11 +3275,11 @@
         <v>24</v>
       </c>
       <c r="G47">
-        <f>A47-F47</f>
+        <f t="shared" si="2"/>
         <v>-22</v>
       </c>
       <c r="J47" s="4">
-        <f>H47*I47</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3252,11 +3301,11 @@
         <v>25</v>
       </c>
       <c r="G48">
-        <f>A48-F48</f>
+        <f t="shared" si="2"/>
         <v>-22</v>
       </c>
       <c r="J48" s="4">
-        <f>H48*I48</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3278,11 +3327,11 @@
         <v>5</v>
       </c>
       <c r="G49">
-        <f>A49-F49</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="J49" s="4">
-        <f>H49*I49</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3304,11 +3353,11 @@
         <v>25</v>
       </c>
       <c r="G50">
-        <f>A50-F50</f>
+        <f t="shared" si="2"/>
         <v>-15</v>
       </c>
       <c r="J50" s="4">
-        <f>H50*I50</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3327,11 +3376,11 @@
         <v>9</v>
       </c>
       <c r="G51">
-        <f>A51-F51</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J51" s="4">
-        <f>H51*I51</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3348,11 +3397,11 @@
         <v>14</v>
       </c>
       <c r="G52">
-        <f t="shared" ref="G37:G68" si="2">A52-F52</f>
+        <f t="shared" ref="G52:G63" si="4">A52-F52</f>
         <v>8</v>
       </c>
       <c r="J52" s="4">
-        <f t="shared" ref="J37:J68" si="3">H52*I52</f>
+        <f t="shared" ref="J52:J63" si="5">H52*I52</f>
         <v>0</v>
       </c>
     </row>
@@ -3374,11 +3423,11 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="J53" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3400,11 +3449,11 @@
         <v>59</v>
       </c>
       <c r="G54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-57</v>
       </c>
       <c r="J54" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3426,11 +3475,11 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J55" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3452,11 +3501,11 @@
         <v>3</v>
       </c>
       <c r="G56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="J56" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3478,18 +3527,18 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J57" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <f>Laptimer!A26*BOM!B2+'Laptimer Remote'!A21*BOM!C2+'CPU Board'!A23*BOM!F2</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B58"/>
       <c r="C58" t="s">
@@ -3502,11 +3551,11 @@
         <v>0</v>
       </c>
       <c r="G58">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>17</v>
       </c>
       <c r="J58" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3526,11 +3575,11 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J59" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3552,11 +3601,11 @@
         <v>3</v>
       </c>
       <c r="G60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J60" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3578,11 +3627,11 @@
         <v>5</v>
       </c>
       <c r="G61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="J61" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3604,11 +3653,11 @@
         <v>1</v>
       </c>
       <c r="G62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J62" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3630,11 +3679,11 @@
         <v>1</v>
       </c>
       <c r="G63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J63" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3724,11 +3773,11 @@
         <v>100</v>
       </c>
       <c r="G68">
-        <f t="shared" ref="G68:G72" si="4">A68-F68</f>
+        <f t="shared" ref="G68:G72" si="6">A68-F68</f>
         <v>-99</v>
       </c>
       <c r="J68" s="4">
-        <f t="shared" ref="J68:J72" si="5">H68*I68</f>
+        <f t="shared" ref="J68:J72" si="7">H68*I68</f>
         <v>0</v>
       </c>
     </row>
@@ -3750,11 +3799,11 @@
         <v>0</v>
       </c>
       <c r="G69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="J69" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3776,11 +3825,11 @@
         <v>20</v>
       </c>
       <c r="G70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-18</v>
       </c>
       <c r="J70" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3802,11 +3851,11 @@
         <v>20</v>
       </c>
       <c r="G71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-18</v>
       </c>
       <c r="J71" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3828,11 +3877,11 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J72" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3854,18 +3903,18 @@
         <v>45</v>
       </c>
       <c r="G73">
-        <f t="shared" ref="G73:G75" si="6">A73-F73</f>
+        <f t="shared" ref="G73:G75" si="8">A73-F73</f>
         <v>-43</v>
       </c>
       <c r="J73" s="4">
-        <f t="shared" ref="J73:J75" si="7">H73*I73</f>
+        <f t="shared" ref="J73:J75" si="9">H73*I73</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <f>'Com Node'!A19*BOM!D2+Relay!A7*BOM!G2+'CPU Board'!A15*BOM!F2</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B74"/>
       <c r="C74" t="s">
@@ -3878,11 +3927,11 @@
         <v>29</v>
       </c>
       <c r="G74">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="8"/>
+        <v>8</v>
       </c>
       <c r="J74" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3902,11 +3951,11 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="J75" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3928,11 +3977,11 @@
         <v>0</v>
       </c>
       <c r="G76">
-        <f t="shared" ref="G76:G78" si="8">A76-F76</f>
+        <f t="shared" ref="G76:G78" si="10">A76-F76</f>
         <v>2</v>
       </c>
       <c r="J76" s="4">
-        <f t="shared" ref="J76:J78" si="9">H76*I76</f>
+        <f t="shared" ref="J76:J78" si="11">H76*I76</f>
         <v>0</v>
       </c>
     </row>
@@ -3952,11 +4001,11 @@
         <v>13</v>
       </c>
       <c r="G77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="J77" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3976,11 +4025,11 @@
         <v>0</v>
       </c>
       <c r="G78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="J78" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4000,11 +4049,11 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <f t="shared" ref="G79" si="10">A79-F79</f>
+        <f t="shared" ref="G79" si="12">A79-F79</f>
         <v>4</v>
       </c>
       <c r="J79" s="4">
-        <f t="shared" ref="J79" si="11">H79*I79</f>
+        <f t="shared" ref="J79" si="13">H79*I79</f>
         <v>0</v>
       </c>
     </row>
@@ -4026,11 +4075,11 @@
         <v>10</v>
       </c>
       <c r="G80">
-        <f t="shared" ref="G80" si="12">A80-F80</f>
+        <f t="shared" ref="G80" si="14">A80-F80</f>
         <v>-8</v>
       </c>
       <c r="J80" s="4">
-        <f t="shared" ref="J80" si="13">H80*I80</f>
+        <f t="shared" ref="J80" si="15">H80*I80</f>
         <v>0</v>
       </c>
     </row>
@@ -4052,11 +4101,11 @@
         <v>0</v>
       </c>
       <c r="G81">
-        <f t="shared" ref="G81:G82" si="14">A81-F81</f>
+        <f t="shared" ref="G81:G82" si="16">A81-F81</f>
         <v>12</v>
       </c>
       <c r="J81" s="4">
-        <f t="shared" ref="J81:J82" si="15">H81*I81</f>
+        <f t="shared" ref="J81:J82" si="17">H81*I81</f>
         <v>0</v>
       </c>
     </row>
@@ -4076,11 +4125,11 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="J82" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4144,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <f>A86-F86</f>
+        <f t="shared" ref="G86:G107" si="18">A86-F86</f>
         <v>4</v>
       </c>
       <c r="J86" s="4">
@@ -4170,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="G87">
-        <f>A87-F87</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J87" s="4">
@@ -4196,7 +4245,7 @@
         <v>0</v>
       </c>
       <c r="G88">
-        <f>A88-F88</f>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="J88" s="4">
@@ -4222,7 +4271,7 @@
         <v>3</v>
       </c>
       <c r="G89">
-        <f>A89-F89</f>
+        <f t="shared" si="18"/>
         <v>-2</v>
       </c>
       <c r="J89" s="4">
@@ -4248,11 +4297,11 @@
         <v>4</v>
       </c>
       <c r="G90">
-        <f>A90-F90</f>
+        <f t="shared" si="18"/>
         <v>-2</v>
       </c>
       <c r="J90" s="4">
-        <f>H90*I90</f>
+        <f t="shared" ref="J90:J107" si="19">H90*I90</f>
         <v>0</v>
       </c>
     </row>
@@ -4274,11 +4323,11 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <f>A91-F91</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J91" s="4">
-        <f>H91*I91</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4300,11 +4349,11 @@
         <v>6</v>
       </c>
       <c r="G92">
-        <f>A92-F92</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J92" s="4">
-        <f>H92*I92</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4324,11 +4373,11 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <f>A93-F93</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="J93" s="4">
-        <f>H93*I93</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4350,18 +4399,18 @@
         <v>2</v>
       </c>
       <c r="G94">
-        <f>A94-F94</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J94" s="4">
-        <f>H94*I94</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <f>'Com Node'!A22*BOM!D2+'CPU Board'!A16*BOM!F2+TC!A19*BOM!I2</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B95" t="s">
         <v>117</v>
@@ -4376,11 +4425,11 @@
         <v>4</v>
       </c>
       <c r="G95">
-        <f>A95-F95</f>
-        <v>10</v>
+        <f t="shared" si="18"/>
+        <v>15</v>
       </c>
       <c r="J95" s="4">
-        <f>H95*I95</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4402,11 +4451,11 @@
         <v>8</v>
       </c>
       <c r="G96">
-        <f>A96-F96</f>
+        <f t="shared" si="18"/>
         <v>-4</v>
       </c>
       <c r="J96" s="4">
-        <f>H96*I96</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4428,11 +4477,11 @@
         <v>2</v>
       </c>
       <c r="G97">
-        <f>A97-F97</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J97" s="4">
-        <f>H97*I97</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4454,11 +4503,11 @@
         <v>0</v>
       </c>
       <c r="G98">
-        <f>A98-F98</f>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="J98" s="4">
-        <f>H98*I98</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4480,11 +4529,11 @@
         <v>0</v>
       </c>
       <c r="G99">
-        <f>A99-F99</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J99" s="4">
-        <f>H99*I99</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4506,11 +4555,11 @@
         <v>0</v>
       </c>
       <c r="G100">
-        <f>A100-F100</f>
+        <f t="shared" si="18"/>
         <v>30</v>
       </c>
       <c r="J100" s="4">
-        <f>H100*I100</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4532,18 +4581,18 @@
         <v>9</v>
       </c>
       <c r="G101">
-        <f>A101-F101</f>
+        <f t="shared" si="18"/>
         <v>-7</v>
       </c>
       <c r="J101" s="4">
-        <f>H101*I101</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <f>Laptimer!A27*BOM!B2+'Laptimer Remote'!A22*BOM!C2+'CPU Board'!A24*BOM!F2</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
         <v>52</v>
@@ -4558,11 +4607,11 @@
         <v>5</v>
       </c>
       <c r="G102">
-        <f>A102-F102</f>
-        <v>7</v>
+        <f t="shared" si="18"/>
+        <v>12</v>
       </c>
       <c r="J102" s="4">
-        <f>H102*I102</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4584,18 +4633,18 @@
         <v>4</v>
       </c>
       <c r="G103">
-        <f>A103-F103</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J103" s="4">
-        <f>H103*I103</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <f>'CPU Board'!A28*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B104"/>
       <c r="C104" t="s">
@@ -4608,11 +4657,11 @@
         <v>6</v>
       </c>
       <c r="G104">
-        <f>A104-F104</f>
-        <v>4</v>
+        <f t="shared" si="18"/>
+        <v>9</v>
       </c>
       <c r="J104" s="4">
-        <f>H104*I104</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4634,11 +4683,11 @@
         <v>4</v>
       </c>
       <c r="G105">
-        <f>A105-F105</f>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="J105" s="4">
-        <f>H105*I105</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4658,11 +4707,11 @@
         <v>0</v>
       </c>
       <c r="G106">
-        <f>A106-F106</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J106" s="4">
-        <f>H106*I106</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4684,11 +4733,11 @@
         <v>0</v>
       </c>
       <c r="G107">
-        <f>A107-F107</f>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="J107" s="4">
-        <f>H107*I107</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4776,18 +4825,18 @@
         <v>10</v>
       </c>
       <c r="G112">
-        <f t="shared" ref="G112:G115" si="16">A112-F112</f>
+        <f t="shared" ref="G112:G115" si="20">A112-F112</f>
         <v>-8</v>
       </c>
       <c r="J112" s="4">
-        <f t="shared" ref="J112:J115" si="17">H112*I112</f>
+        <f t="shared" ref="J112:J115" si="21">H112*I112</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <f>Laptimer!A23*BOM!B2+'Laptimer Remote'!A18*BOM!C2+'CPU Board'!A18*BOM!F2</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
         <v>56</v>
@@ -4802,18 +4851,18 @@
         <v>8</v>
       </c>
       <c r="G113">
-        <f t="shared" si="16"/>
-        <v>4</v>
+        <f t="shared" si="20"/>
+        <v>9</v>
       </c>
       <c r="J113" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <f>Laptimer!A41*BOM!B2+'CPU Board'!A30*BOM!F2</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B114" t="s">
         <v>80</v>
@@ -4824,12 +4873,15 @@
       <c r="D114" t="s">
         <v>55</v>
       </c>
+      <c r="F114" s="4">
+        <v>7</v>
+      </c>
       <c r="G114">
-        <f t="shared" si="16"/>
-        <v>11</v>
+        <f t="shared" si="20"/>
+        <v>9</v>
       </c>
       <c r="J114" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -4847,12 +4899,15 @@
       <c r="D115" t="s">
         <v>59</v>
       </c>
+      <c r="F115" s="4">
+        <v>2</v>
+      </c>
       <c r="G115">
-        <f t="shared" si="16"/>
-        <v>2</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="J115" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -4870,12 +4925,15 @@
       <c r="D116" t="s">
         <v>105</v>
       </c>
+      <c r="F116" s="4">
+        <v>0</v>
+      </c>
       <c r="G116">
-        <f t="shared" ref="G116:G118" si="18">A116-F116</f>
+        <f t="shared" ref="G116:G118" si="22">A116-F116</f>
         <v>2</v>
       </c>
       <c r="J116" s="4">
-        <f t="shared" ref="J116:J118" si="19">H116*I116</f>
+        <f t="shared" ref="J116:J118" si="23">H116*I116</f>
         <v>0</v>
       </c>
     </row>
@@ -4893,12 +4951,15 @@
       <c r="D117" t="s">
         <v>131</v>
       </c>
+      <c r="F117" s="4">
+        <v>7</v>
+      </c>
       <c r="G117">
-        <f t="shared" si="18"/>
-        <v>2</v>
+        <f t="shared" si="22"/>
+        <v>-5</v>
       </c>
       <c r="J117" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -4914,12 +4975,15 @@
       <c r="D118" t="s">
         <v>133</v>
       </c>
+      <c r="F118" s="4">
+        <v>0</v>
+      </c>
       <c r="G118">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="J118" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -4937,12 +5001,15 @@
       <c r="D119" t="s">
         <v>137</v>
       </c>
+      <c r="F119" s="4">
+        <v>0</v>
+      </c>
       <c r="G119">
-        <f t="shared" ref="G119:G121" si="20">A119-F119</f>
+        <f t="shared" ref="G119:G121" si="24">A119-F119</f>
         <v>2</v>
       </c>
       <c r="J119" s="4">
-        <f t="shared" ref="J119:J121" si="21">H119*I119</f>
+        <f t="shared" ref="J119:J121" si="25">H119*I119</f>
         <v>0</v>
       </c>
     </row>
@@ -4960,12 +5027,15 @@
       <c r="D120" t="s">
         <v>139</v>
       </c>
+      <c r="F120" s="4">
+        <v>23</v>
+      </c>
       <c r="G120">
-        <f t="shared" si="20"/>
-        <v>12</v>
+        <f t="shared" si="24"/>
+        <v>-11</v>
       </c>
       <c r="J120" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -4983,12 +5053,15 @@
       <c r="D121" t="s">
         <v>145</v>
       </c>
+      <c r="F121" s="4">
+        <v>0</v>
+      </c>
       <c r="G121">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="J121" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -5006,12 +5079,15 @@
       <c r="D122" t="s">
         <v>148</v>
       </c>
+      <c r="F122" s="4">
+        <v>0</v>
+      </c>
       <c r="G122">
         <f>A122-F122</f>
         <v>2</v>
       </c>
       <c r="J122" s="4">
-        <f t="shared" ref="J122" si="22">H122*I122</f>
+        <f t="shared" ref="J122" si="26">H122*I122</f>
         <v>0</v>
       </c>
     </row>
@@ -5029,19 +5105,22 @@
       <c r="D123" t="s">
         <v>166</v>
       </c>
+      <c r="F123" s="4">
+        <v>0</v>
+      </c>
       <c r="G123">
         <f>A123-F123</f>
         <v>2</v>
       </c>
       <c r="J123" s="4">
-        <f t="shared" ref="J123" si="23">H123*I123</f>
+        <f t="shared" ref="J123" si="27">H123*I123</f>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
         <f>'CPU Board'!A2*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B124" t="s">
         <v>179</v>
@@ -5052,19 +5131,22 @@
       <c r="D124" t="s">
         <v>175</v>
       </c>
+      <c r="F124" s="4">
+        <v>3</v>
+      </c>
       <c r="G124">
-        <f t="shared" ref="G124:G129" si="24">A124-F124</f>
-        <v>10</v>
+        <f t="shared" ref="G124:G129" si="28">A124-F124</f>
+        <v>12</v>
       </c>
       <c r="J124" s="4">
-        <f t="shared" ref="J124:J129" si="25">H124*I124</f>
+        <f t="shared" ref="J124:J129" si="29">H124*I124</f>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
         <f>'CPU Board'!A3*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B125" t="s">
         <v>176</v>
@@ -5075,19 +5157,22 @@
       <c r="D125" t="s">
         <v>178</v>
       </c>
+      <c r="F125" s="4">
+        <v>0</v>
+      </c>
       <c r="G125">
-        <f t="shared" si="24"/>
-        <v>10</v>
+        <f t="shared" si="28"/>
+        <v>15</v>
       </c>
       <c r="J125" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
         <f>'CPU Board'!A17*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B126" t="s">
         <v>192</v>
@@ -5098,19 +5183,22 @@
       <c r="D126" t="s">
         <v>191</v>
       </c>
+      <c r="F126" s="4">
+        <v>0</v>
+      </c>
       <c r="G126">
-        <f t="shared" si="24"/>
-        <v>10</v>
+        <f t="shared" si="28"/>
+        <v>15</v>
       </c>
       <c r="J126" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127">
         <f>'CPU Board'!A20*BOM!F2</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B127"/>
       <c r="C127" t="s">
@@ -5119,19 +5207,22 @@
       <c r="D127" t="s">
         <v>197</v>
       </c>
+      <c r="F127" s="4">
+        <v>0</v>
+      </c>
       <c r="G127">
-        <f t="shared" si="24"/>
-        <v>20</v>
+        <f t="shared" si="28"/>
+        <v>30</v>
       </c>
       <c r="J127" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
         <f>'CPU Board'!A21*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B128"/>
       <c r="C128" t="s">
@@ -5140,19 +5231,22 @@
       <c r="D128" t="s">
         <v>195</v>
       </c>
+      <c r="F128" s="4">
+        <v>0</v>
+      </c>
       <c r="G128">
-        <f t="shared" si="24"/>
-        <v>10</v>
+        <f t="shared" si="28"/>
+        <v>15</v>
       </c>
       <c r="J128" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <f>'CPU Board'!A22*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B129"/>
       <c r="C129" t="s">
@@ -5161,19 +5255,22 @@
       <c r="D129" t="s">
         <v>193</v>
       </c>
+      <c r="F129" s="4">
+        <v>0</v>
+      </c>
       <c r="G129">
-        <f t="shared" si="24"/>
-        <v>10</v>
+        <f t="shared" si="28"/>
+        <v>15</v>
       </c>
       <c r="J129" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <f>'CPU Board'!A29*BOM!F2+TC!A39*BOM!I2</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B130" t="s">
         <v>205</v>
@@ -5184,19 +5281,22 @@
       <c r="D130" t="s">
         <v>204</v>
       </c>
+      <c r="F130" s="4">
+        <v>6</v>
+      </c>
       <c r="G130">
-        <f t="shared" ref="G130:G131" si="26">A130-F130</f>
-        <v>18</v>
+        <f t="shared" ref="G130:G131" si="30">A130-F130</f>
+        <v>17</v>
       </c>
       <c r="J130" s="4">
-        <f t="shared" ref="J130:J131" si="27">H130*I130</f>
+        <f t="shared" ref="J130:J131" si="31">H130*I130</f>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <f>'CPU Board'!A31*BOM!F2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B131"/>
       <c r="C131" t="s">
@@ -5205,12 +5305,15 @@
       <c r="D131" t="s">
         <v>206</v>
       </c>
+      <c r="F131" s="4">
+        <v>0</v>
+      </c>
       <c r="G131">
-        <f t="shared" si="26"/>
-        <v>10</v>
+        <f t="shared" si="30"/>
+        <v>15</v>
       </c>
       <c r="J131" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -5228,12 +5331,15 @@
       <c r="D132" t="s">
         <v>210</v>
       </c>
+      <c r="F132" s="4">
+        <v>0</v>
+      </c>
       <c r="G132">
-        <f t="shared" ref="G132:G136" si="28">A132-F132</f>
+        <f t="shared" ref="G132:G134" si="32">A132-F132</f>
         <v>4</v>
       </c>
       <c r="J132" s="4">
-        <f t="shared" ref="J132:J136" si="29">H132*I132</f>
+        <f t="shared" ref="J132:J134" si="33">H132*I132</f>
         <v>0</v>
       </c>
     </row>
@@ -5251,12 +5357,15 @@
       <c r="D133" t="s">
         <v>209</v>
       </c>
+      <c r="F133" s="4">
+        <v>0</v>
+      </c>
       <c r="G133">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="J133" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -5266,7 +5375,7 @@
         <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="C134" t="s">
         <v>208</v>
@@ -5274,445 +5383,538 @@
       <c r="D134" t="s">
         <v>208</v>
       </c>
+      <c r="F134" s="4">
+        <v>0</v>
+      </c>
       <c r="G134">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="J134" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135">
+      <c r="A135" s="4">
+        <f>A134</f>
+        <v>2</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="F135" s="4">
+        <v>1</v>
+      </c>
+      <c r="G135">
+        <f t="shared" ref="G135" si="34">A135-F135</f>
+        <v>1</v>
+      </c>
+      <c r="J135" s="4">
+        <f t="shared" ref="J135" si="35">H135*I135</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136">
         <f>Relay!A6*BOM!G2</f>
         <v>8</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B136" t="s">
         <v>213</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>213</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D136" t="s">
         <v>214</v>
       </c>
-      <c r="G135">
-        <f t="shared" si="28"/>
-        <v>8</v>
-      </c>
-      <c r="J135" s="4">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136">
+      <c r="F136" s="4">
+        <v>2</v>
+      </c>
+      <c r="G136">
+        <f>A136-F136</f>
+        <v>6</v>
+      </c>
+      <c r="J136" s="4">
+        <f>H136*I136</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137">
         <f>Relay!A8*BOM!G2</f>
         <v>8</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>212</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>212</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>211</v>
       </c>
-      <c r="G136">
-        <f t="shared" si="28"/>
-        <v>8</v>
-      </c>
-      <c r="J136" s="4">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <f>'H-bridge'!A2*BOM!H2</f>
-        <v>2</v>
-      </c>
-      <c r="B137" t="s">
-        <v>216</v>
-      </c>
-      <c r="C137" t="s">
-        <v>216</v>
-      </c>
-      <c r="D137" t="s">
-        <v>216</v>
+      <c r="F137" s="4">
+        <v>1</v>
       </c>
       <c r="G137">
-        <f t="shared" ref="G137:G140" si="30">A137-F137</f>
-        <v>2</v>
+        <f>A137-F137</f>
+        <v>7</v>
       </c>
       <c r="J137" s="4">
-        <f t="shared" ref="J137:J140" si="31">H137*I137</f>
+        <f>H137*I137</f>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
+        <f>'H-bridge'!A2*BOM!H2</f>
+        <v>2</v>
+      </c>
+      <c r="B138" t="s">
+        <v>216</v>
+      </c>
+      <c r="C138" t="s">
+        <v>216</v>
+      </c>
+      <c r="D138" t="s">
+        <v>216</v>
+      </c>
+      <c r="F138" s="4">
+        <v>0</v>
+      </c>
+      <c r="G138">
+        <f t="shared" ref="G138:G140" si="36">A138-F138</f>
+        <v>2</v>
+      </c>
+      <c r="J138" s="4">
+        <f t="shared" ref="J138:J141" si="37">H138*I138</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139">
         <f>'H-bridge'!A7*BOM!H2</f>
         <v>8</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" t="s">
         <v>221</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C139" t="s">
         <v>221</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D139" t="s">
         <v>220</v>
       </c>
-      <c r="G138">
-        <f t="shared" si="30"/>
+      <c r="F139" s="4">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <f t="shared" si="36"/>
         <v>8</v>
       </c>
-      <c r="J138" s="4">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139">
+      <c r="J139" s="4">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140">
         <f>TC!A5*BOM!I2</f>
         <v>4</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>228</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C140" t="s">
+        <v>502</v>
+      </c>
+      <c r="D140" t="s">
         <v>227</v>
       </c>
-      <c r="D139" t="s">
+      <c r="F140" s="4">
+        <v>1</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="36"/>
+        <v>3</v>
+      </c>
+      <c r="J140" s="4">
+        <f>H140*I140</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>0</v>
+      </c>
+      <c r="B141" t="s">
+        <v>241</v>
+      </c>
+      <c r="C141" t="s">
+        <v>79</v>
+      </c>
+      <c r="D141" t="s">
+        <v>78</v>
+      </c>
+      <c r="F141" s="4">
+        <v>2</v>
+      </c>
+      <c r="G141">
+        <f t="shared" ref="G141:G142" si="38">A141-F141</f>
+        <v>-2</v>
+      </c>
+      <c r="J141" s="4">
+        <f t="shared" ref="J141:J143" si="39">H141*I141</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" s="4">
+        <f>A140</f>
+        <v>4</v>
+      </c>
+      <c r="B142" t="s">
+        <v>228</v>
+      </c>
+      <c r="C142" t="s">
         <v>227</v>
       </c>
-      <c r="G139">
-        <f t="shared" si="30"/>
+      <c r="D142" t="s">
+        <v>227</v>
+      </c>
+      <c r="F142" s="4">
+        <v>2</v>
+      </c>
+      <c r="G142">
+        <f>A142-F142</f>
+        <v>2</v>
+      </c>
+      <c r="J142" s="4">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <f>A136</f>
+        <v>8</v>
+      </c>
+      <c r="B143" t="s">
+        <v>503</v>
+      </c>
+      <c r="C143" t="s">
+        <v>504</v>
+      </c>
+      <c r="D143" t="s">
+        <v>214</v>
+      </c>
+      <c r="F143" s="4">
+        <v>3</v>
+      </c>
+      <c r="G143">
+        <f>A143-F143</f>
+        <v>5</v>
+      </c>
+      <c r="J143" s="4">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I145" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J145" s="6">
+        <f>SUM(J111:J115)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A147" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E147" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J139" s="4">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <v>0</v>
-      </c>
-      <c r="B140" t="s">
-        <v>241</v>
-      </c>
-      <c r="C140" t="s">
-        <v>79</v>
-      </c>
-      <c r="D140" t="s">
-        <v>78</v>
-      </c>
-      <c r="G140">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="J140" s="4">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I141" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J141" s="6">
-        <f>SUM(J111:J115)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:10" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A143" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E143" s="3" t="s">
+      <c r="F147" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <f>Laptimer!A15*BOM!B2</f>
+        <v>1</v>
+      </c>
+      <c r="B148" t="s">
+        <v>499</v>
+      </c>
+      <c r="C148" t="s">
+        <v>61</v>
+      </c>
+      <c r="D148" t="s">
+        <v>62</v>
+      </c>
+      <c r="F148" s="4">
         <v>4</v>
       </c>
-      <c r="F143" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G143" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H143" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I143" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J143" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <f>Laptimer!A15*BOM!B2</f>
-        <v>1</v>
-      </c>
-      <c r="B144" t="s">
-        <v>499</v>
-      </c>
-      <c r="C144" t="s">
-        <v>61</v>
-      </c>
-      <c r="D144" t="s">
-        <v>62</v>
-      </c>
-      <c r="F144" s="4">
-        <v>4</v>
-      </c>
-      <c r="G144">
-        <f>A144-F144</f>
+      <c r="G148">
+        <f>A148-F148</f>
         <v>-3</v>
       </c>
-      <c r="J144" s="4">
-        <f>H144*I144</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145">
+      <c r="J148" s="4">
+        <f>H148*I148</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A149">
         <f>Laptimer!A19*BOM!B2+'Laptimer Remote'!A13*BOM!C2+'Com Node'!A17*BOM!D2</f>
         <v>4</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B149" t="s">
         <v>82</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C149" t="s">
         <v>82</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D149" t="s">
         <v>81</v>
       </c>
-      <c r="F145" s="4">
-        <v>0</v>
-      </c>
-      <c r="G145">
-        <f t="shared" ref="G145:G147" si="32">A145-F145</f>
+      <c r="F149" s="4">
+        <v>0</v>
+      </c>
+      <c r="G149">
+        <f t="shared" ref="G149:G151" si="40">A149-F149</f>
         <v>4</v>
       </c>
-      <c r="J145" s="4">
-        <f t="shared" ref="J145:J147" si="33">H145*I145</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146">
+      <c r="J149" s="4">
+        <f t="shared" ref="J149:J151" si="41">H149*I149</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150">
         <f>Laptimer!A45*BOM!B2+'Com Node'!A47*BOM!D2</f>
         <v>3</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B150" t="s">
         <v>63</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C150" t="s">
         <v>63</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D150" t="s">
         <v>63</v>
       </c>
-      <c r="F146" s="4">
-        <v>2</v>
-      </c>
-      <c r="G146">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="J146" s="4">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A147">
+      <c r="F150" s="4">
+        <v>2</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="J150" s="4">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151">
         <f>'Com Node'!A2*BOM!D2</f>
         <v>2</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="C151" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D147" s="4" t="s">
+      <c r="D151" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F147" s="4">
-        <v>0</v>
-      </c>
-      <c r="G147">
-        <f t="shared" si="32"/>
-        <v>2</v>
-      </c>
-      <c r="J147" s="4">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A148">
+      <c r="F151" s="4">
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="40"/>
+        <v>2</v>
+      </c>
+      <c r="J151" s="4">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152">
         <f>'Com Node'!A15*BOM!D2</f>
         <v>4</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B152" t="s">
         <v>104</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C152" t="s">
         <v>61</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D152" t="s">
         <v>62</v>
       </c>
-      <c r="F148" s="4">
-        <v>0</v>
-      </c>
-      <c r="G148">
-        <f>A148-F148</f>
+      <c r="F152" s="4">
+        <v>0</v>
+      </c>
+      <c r="G152">
+        <f>A152-F152</f>
         <v>4</v>
       </c>
-      <c r="J148" s="4">
-        <f>H148*I148</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A149">
+      <c r="J152" s="4">
+        <f>H152*I152</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A153">
         <f>Dashboard!A12*BOM!E2</f>
         <v>2</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B153" t="s">
         <v>158</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C153" t="s">
         <v>158</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D153" t="s">
         <v>158</v>
       </c>
-      <c r="F149" s="4">
-        <v>0</v>
-      </c>
-      <c r="G149">
-        <f t="shared" ref="G149:G150" si="34">A149-F149</f>
-        <v>2</v>
-      </c>
-      <c r="J149" s="4">
-        <f t="shared" ref="J149:J150" si="35">H149*I149</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <f>A149</f>
-        <v>2</v>
-      </c>
-      <c r="B150" t="s">
+      <c r="F153" s="4">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <f t="shared" ref="G153:G154" si="42">A153-F153</f>
+        <v>2</v>
+      </c>
+      <c r="J153" s="4">
+        <f t="shared" ref="J153:J154" si="43">H153*I153</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <f>A153</f>
+        <v>2</v>
+      </c>
+      <c r="B154" t="s">
         <v>159</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C154" t="s">
         <v>158</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D154" t="s">
         <v>158</v>
       </c>
-      <c r="F150" s="4">
-        <v>0</v>
-      </c>
-      <c r="G150">
-        <f t="shared" si="34"/>
-        <v>2</v>
-      </c>
-      <c r="J150" s="4">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151">
+      <c r="F154" s="4">
+        <v>0</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="42"/>
+        <v>2</v>
+      </c>
+      <c r="J154" s="4">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155">
         <f>'CPU Board'!A13*BOM!F2</f>
-        <v>10</v>
-      </c>
-      <c r="B151" t="s">
+        <v>15</v>
+      </c>
+      <c r="B155" t="s">
         <v>185</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C155" t="s">
         <v>186</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D155" t="s">
         <v>187</v>
       </c>
-      <c r="E151"/>
-      <c r="F151" s="9">
-        <v>1</v>
-      </c>
-      <c r="G151">
-        <f t="shared" ref="G151" si="36">A151-F151</f>
-        <v>9</v>
-      </c>
-      <c r="J151" s="4">
-        <f t="shared" ref="J151" si="37">H151*I151</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A152">
+      <c r="E155"/>
+      <c r="F155" s="9">
+        <v>1</v>
+      </c>
+      <c r="G155">
+        <f t="shared" ref="G155" si="44">A155-F155</f>
+        <v>14</v>
+      </c>
+      <c r="J155" s="4">
+        <f t="shared" ref="J155" si="45">H155*I155</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156">
         <f>'CPU Board'!A14*BOM!F2</f>
-        <v>10</v>
-      </c>
-      <c r="B152" t="s">
+        <v>15</v>
+      </c>
+      <c r="B156" t="s">
         <v>188</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C156" t="s">
         <v>189</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D156" t="s">
         <v>190</v>
       </c>
-      <c r="F152" s="4">
+      <c r="F156" s="4">
         <v>7</v>
       </c>
-      <c r="G152">
-        <f t="shared" ref="G152" si="38">A152-F152</f>
-        <v>3</v>
-      </c>
-      <c r="J152" s="4">
-        <f t="shared" ref="J152" si="39">H152*I152</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I153" s="4" t="s">
+      <c r="G156">
+        <f t="shared" ref="G156" si="46">A156-F156</f>
+        <v>8</v>
+      </c>
+      <c r="J156" s="4">
+        <f t="shared" ref="J156" si="47">H156*I156</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I157" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J153" s="6">
-        <f>SUM(J144:J152)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="155" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J155" s="7">
-        <f>J153+J141+J108+J83+J64</f>
-        <v>0</v>
-      </c>
-      <c r="K155" t="s">
+      <c r="J157" s="6">
+        <f>SUM(J148:J156)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J159" s="7">
+        <f>J157+J145+J108+J83+J64</f>
+        <v>0</v>
+      </c>
+      <c r="K159" t="s">
         <v>245</v>
       </c>
     </row>
@@ -5721,21 +5923,42 @@
     <sortCondition ref="C86:C107"/>
   </sortState>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
+  <conditionalFormatting sqref="A145:XFD160 A141:E141 H141:I141 F141:G143 K141:XFD141 J141:J143 A1:XFD134 A136:XFD140 F135:J135">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A161:XFD1048576">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G148:G156 G86:G107 G67:G82 G5:G63 G111:G143">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G148:G156 G86:G107 G67:G82 G5:G63 G111:G143">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B142:D142">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A143:D143">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Final order for RS + missing things from farnell
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Documents\GitHub\g5-pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAU Racing\g5-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="600">
   <si>
     <t>Pass</t>
   </si>
@@ -1790,6 +1790,48 @@
   </si>
   <si>
     <t>http://dk.rs-online.com/web/p/koretojsstik/7239359/</t>
+  </si>
+  <si>
+    <t>jtag 6</t>
+  </si>
+  <si>
+    <t>2 pin</t>
+  </si>
+  <si>
+    <t>can arm</t>
+  </si>
+  <si>
+    <t>white clic 2</t>
+  </si>
+  <si>
+    <t>white clicl 3</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>kun uden vinkel</t>
+  </si>
+  <si>
+    <t>y/n</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/molex/39-30-0040/header-mini-fit-r-a-dual-row-4way/dp/1697133</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/molex/39-30-1060/header-right-angle-dual-row-6/dp/9963383</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/molex/22-05-7028/connector-header-tht-ra-2-54mm/dp/9731601</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/multicomp/2214s-22sg-85/socket-pcb-2-row-vert-22way/dp/1593495</t>
+  </si>
+  <si>
+    <t>20 købt</t>
   </si>
 </sst>
 </file>
@@ -1836,7 +1878,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1858,6 +1900,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1914,7 +1962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1930,6 +1978,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2316,10 +2366,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="M153" sqref="M153"/>
+      <selection pane="bottomLeft" activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2995,11 +3045,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="L25" s="13" t="s">
         <v>571</v>
       </c>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12" t="s">
+      <c r="M25" s="13"/>
+      <c r="N25" s="13" t="s">
         <v>525</v>
       </c>
     </row>
@@ -4046,8 +4096,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:12" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:14" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>33</v>
       </c>
@@ -4079,7 +4129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <f>Laptimer!A5*BOM!B2+'Laptimer Remote'!A3*BOM!C2</f>
         <v>6</v>
@@ -4105,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <f>Laptimer!A16*BOM!B2</f>
         <v>1</v>
@@ -4131,7 +4181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>Laptimer!A17*BOM!B2+'Laptimer Remote'!A11*BOM!C2</f>
         <v>2</v>
@@ -4157,7 +4207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <f>Laptimer!A40*BOM!B2+'Laptimer Remote'!A32*BOM!C2</f>
         <v>2</v>
@@ -4183,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>Laptimer!A43*BOM!B2+'Laptimer Remote'!A34*BOM!C2</f>
         <v>2</v>
@@ -4209,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <f>'Laptimer Remote'!A12*BOM!C2</f>
         <v>1</v>
@@ -4241,7 +4291,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <f>'Com Node'!A3*BOM!D2</f>
         <v>2</v>
@@ -4267,7 +4317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <f>'Com Node'!A19*BOM!D2+Relay!A7*BOM!G2+'CPU Board'!A15*BOM!F2</f>
         <v>37</v>
@@ -4294,7 +4344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <f>'Com Node'!A20*BOM!D2</f>
         <v>8</v>
@@ -4321,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <f>'Com Node'!A42*BOM!D2</f>
         <v>2</v>
@@ -4350,7 +4400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <f>'Com Node'!A46*BOM!D2+TC!A41*BOM!I2</f>
         <v>12</v>
@@ -4377,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <f>Dashboard!A15*BOM!E2</f>
         <v>40</v>
@@ -4403,11 +4453,14 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="L78" s="12" t="s">
+      <c r="L78" s="14" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N78" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <f>Dashboard!A27*BOM!E2+TC!A38*BOM!I2</f>
         <v>4</v>
@@ -4434,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <f>Dashboard!A17*BOM!E2</f>
         <v>2</v>
@@ -4515,7 +4568,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="L82" s="12" t="s">
+      <c r="L82" s="13" t="s">
         <v>525</v>
       </c>
     </row>
@@ -4647,7 +4700,7 @@
         <f>H88*I88</f>
         <v>0</v>
       </c>
-      <c r="L88" s="12" t="s">
+      <c r="L88" s="13" t="s">
         <v>578</v>
       </c>
     </row>
@@ -5248,6 +5301,12 @@
         <f>H111*I111</f>
         <v>0</v>
       </c>
+      <c r="K111" t="s">
+        <v>591</v>
+      </c>
+      <c r="L111" t="s">
+        <v>586</v>
+      </c>
       <c r="M111" t="s">
         <v>529</v>
       </c>
@@ -5474,7 +5533,7 @@
         <f t="shared" ref="J119:J121" si="25">H119*I119</f>
         <v>0</v>
       </c>
-      <c r="M119" s="12" t="s">
+      <c r="M119" s="13" t="s">
         <v>525</v>
       </c>
       <c r="N119" t="s">
@@ -5538,6 +5597,12 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
+      <c r="K121" t="s">
+        <v>591</v>
+      </c>
+      <c r="L121" t="s">
+        <v>587</v>
+      </c>
       <c r="M121" t="s">
         <v>529</v>
       </c>
@@ -5559,6 +5624,9 @@
       <c r="D122" t="s">
         <v>148</v>
       </c>
+      <c r="E122" s="4" t="s">
+        <v>597</v>
+      </c>
       <c r="F122" s="4">
         <v>0</v>
       </c>
@@ -5566,9 +5634,15 @@
         <f>A122-F122</f>
         <v>2</v>
       </c>
-      <c r="J122" s="4">
+      <c r="I122" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="J122" s="4" t="e">
         <f t="shared" ref="J122" si="26">H122*I122</f>
-        <v>0</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K122" t="s">
+        <v>593</v>
       </c>
       <c r="M122" t="s">
         <v>529</v>
@@ -5591,6 +5665,9 @@
       <c r="D123" t="s">
         <v>166</v>
       </c>
+      <c r="E123" s="4" t="s">
+        <v>596</v>
+      </c>
       <c r="F123" s="4">
         <v>0</v>
       </c>
@@ -5602,11 +5679,8 @@
         <f t="shared" ref="J123" si="27">H123*I123</f>
         <v>0</v>
       </c>
-      <c r="M123" t="s">
-        <v>529</v>
-      </c>
-      <c r="O123" t="s">
-        <v>551</v>
+      <c r="K123" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
@@ -5634,6 +5708,9 @@
         <f t="shared" ref="J124:J129" si="29">H124*I124</f>
         <v>0</v>
       </c>
+      <c r="K124" t="s">
+        <v>591</v>
+      </c>
       <c r="L124" t="s">
         <v>552</v>
       </c>
@@ -5687,6 +5764,9 @@
       <c r="D126" t="s">
         <v>191</v>
       </c>
+      <c r="E126" s="4" t="s">
+        <v>595</v>
+      </c>
       <c r="F126" s="4">
         <v>0</v>
       </c>
@@ -5698,11 +5778,11 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="M126" t="s">
-        <v>529</v>
-      </c>
-      <c r="O126" t="s">
-        <v>551</v>
+      <c r="K126" t="s">
+        <v>594</v>
+      </c>
+      <c r="L126" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
@@ -5717,6 +5797,9 @@
       <c r="D127" t="s">
         <v>197</v>
       </c>
+      <c r="E127" s="4" t="s">
+        <v>598</v>
+      </c>
       <c r="F127" s="4">
         <v>0</v>
       </c>
@@ -5728,11 +5811,8 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="M127" t="s">
-        <v>529</v>
-      </c>
-      <c r="O127" t="s">
-        <v>551</v>
+      <c r="K127" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
@@ -5758,6 +5838,9 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
+      <c r="K128" t="s">
+        <v>591</v>
+      </c>
       <c r="M128" t="s">
         <v>529</v>
       </c>
@@ -5788,6 +5871,9 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
+      <c r="K129" t="s">
+        <v>591</v>
+      </c>
       <c r="M129" t="s">
         <v>529</v>
       </c>
@@ -5847,11 +5933,14 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="M131" s="12" t="s">
+      <c r="K131" t="s">
+        <v>591</v>
+      </c>
+      <c r="M131" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="N131" s="12"/>
-      <c r="O131" s="12" t="s">
+      <c r="N131" s="13"/>
+      <c r="O131" s="13" t="s">
         <v>551</v>
       </c>
     </row>
@@ -5880,11 +5969,17 @@
         <f t="shared" ref="J132:J134" si="33">H132*I132</f>
         <v>0</v>
       </c>
-      <c r="M132" s="12" t="s">
+      <c r="K132" t="s">
+        <v>591</v>
+      </c>
+      <c r="L132" t="s">
+        <v>589</v>
+      </c>
+      <c r="M132" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="N132" s="12"/>
-      <c r="O132" s="12" t="s">
+      <c r="N132" s="13"/>
+      <c r="O132" s="13" t="s">
         <v>551</v>
       </c>
     </row>
@@ -5913,11 +6008,17 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="M133" s="12" t="s">
+      <c r="K133" t="s">
+        <v>591</v>
+      </c>
+      <c r="L133" t="s">
+        <v>590</v>
+      </c>
+      <c r="M133" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="N133" s="12"/>
-      <c r="O133" s="12" t="s">
+      <c r="N133" s="13"/>
+      <c r="O133" s="13" t="s">
         <v>551</v>
       </c>
     </row>
@@ -5946,6 +6047,9 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
+      <c r="K134" t="s">
+        <v>591</v>
+      </c>
       <c r="M134" t="s">
         <v>529</v>
       </c>
@@ -5971,6 +6075,9 @@
       <c r="J135" s="4">
         <f t="shared" ref="J135" si="35">H135*I135</f>
         <v>0</v>
+      </c>
+      <c r="K135" t="s">
+        <v>591</v>
       </c>
       <c r="M135" t="s">
         <v>529</v>
@@ -6062,6 +6169,9 @@
         <f t="shared" ref="J138:J139" si="37">H138*I138</f>
         <v>0</v>
       </c>
+      <c r="K138" t="s">
+        <v>591</v>
+      </c>
       <c r="M138" t="s">
         <v>529</v>
       </c>
@@ -6094,6 +6204,9 @@
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
+      <c r="K139" t="s">
+        <v>591</v>
+      </c>
       <c r="M139" t="s">
         <v>529</v>
       </c>
@@ -6129,7 +6242,7 @@
         <f>H140*I140</f>
         <v>0</v>
       </c>
-      <c r="M140" s="12" t="s">
+      <c r="M140" s="13" t="s">
         <v>525</v>
       </c>
     </row>
@@ -6157,6 +6270,7 @@
         <f t="shared" ref="J141:J142" si="39">H141*I141</f>
         <v>0</v>
       </c>
+      <c r="M141" s="13"/>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
@@ -6186,7 +6300,7 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="M142" s="12" t="s">
+      <c r="M142" s="13" t="s">
         <v>525</v>
       </c>
     </row>
@@ -6533,7 +6647,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A144:XFD159 A141:E141 H141:I141 F141:G142 K141:XFD141 J141:J142 A1:XFD24 F135:J135 N25:XFD26 A25:L26 A136:XFD140 M142 A27:XFD134">
+  <conditionalFormatting sqref="A144:XFD159 A141:E141 H141:I141 F141:G142 K141:XFD141 J141:J142 A1:XFD24 N25:XFD26 A25:L26 A136:XFD140 M142 A27:XFD134 F135:K135">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6579,7 +6693,7 @@
   <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -8183,7 +8297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -9120,7 +9234,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9733,7 +9847,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10346,7 +10460,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10785,7 +10899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>